<commit_message>
full reworking of all models
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/carown_LR_new/All.xlsx
+++ b/outputs/ML_Results/carown_LR_new/All.xlsx
@@ -7,14 +7,14 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summ0" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="summ41" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="summ6" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="summ4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="summ15" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="summ1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="summ11" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summ4" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summ3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="summ6" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="summ1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="summ13" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="summ5" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="summ35" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="summ0" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="summ10" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,296 +466,218 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.5867834001394387</v>
+        <v>-0.6792876572187736</v>
       </c>
       <c r="C2" t="n">
-        <v>0.723605681669149</v>
+        <v>0.0001154037508087015</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult]</t>
+          <t>Country[T.Germany]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.142193147475763</v>
+        <v>-0.6932928383871587</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4887616435929946</v>
+        <v>7.389768819826593e-47</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult_Kids]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.313392848637895</v>
+        <v>0.265190506434564</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4263178209297729</v>
+        <v>2.862631531377701e-73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female]</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1027777900519953</v>
+        <v>0.0005603425989494482</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9503400895051579</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.4569590728533451</v>
+        <v>0.01518467287388999</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7818656636962555</v>
+        <v>9.898582073376447e-39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Parent]</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6137110577346329</v>
+        <v>0.01909577362631367</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7100944982358839</v>
+        <v>0.5525966870532008</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Country[T.Germany]</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.8182300725486638</v>
+        <v>0.4207491837138595</v>
       </c>
       <c r="C8" t="n">
-        <v>1.41593897991974e-60</v>
+        <v>4.923493323300056e-19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.02440797545415114</v>
+        <v>0.2460489416724882</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4092265161705243</v>
+        <v>6.490934952455066e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004754076277193764</v>
+        <v>-7.398088470586898e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>6.413785005989011e-279</v>
+        <v>8.321799084141013e-123</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01422733305144655</v>
+        <v>0.006649625420101253</v>
       </c>
       <c r="C11" t="n">
-        <v>3.770503216345371e-32</v>
+        <v>0.4760156776144464</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.009536439432808866</v>
+        <v>-0.001578298991352138</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7696957422350345</v>
+        <v>0.7271301704805967</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5321309480115906</v>
+        <v>0.1927770932598639</v>
       </c>
       <c r="C13" t="n">
-        <v>1.00283908959455e-28</v>
+        <v>0.2308065717258432</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.346470804454285</v>
+        <v>-0.001075451042636122</v>
       </c>
       <c r="C14" t="n">
-        <v>3.554734514424125e-08</v>
+        <v>0.4075118299921993</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7.642993917054636e-05</v>
+        <v>-0.001160357900432417</v>
       </c>
       <c r="C15" t="n">
-        <v>2.460189192038027e-91</v>
+        <v>0.2276299366658003</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.234019914080135e-08</v>
+        <v>0.7798484611914137</v>
       </c>
       <c r="C16" t="n">
-        <v>0.001693052221999848</v>
+        <v>8.123662600689844e-12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.008611024803905996</v>
+        <v>-0.9138947773743836</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3622461522899779</v>
+        <v>1.111752971516955e-10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>transit_accessibility</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.000795787946184722</v>
+        <v>-0.000153784295390177</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8622256539974167</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>bike_lane_share</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.1779458593311608</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.2716064534636566</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>IntersecDensity</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.001031801043201054</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.4318473654314776</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>street_length</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>-0.001689039904435987</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.08412891212678139</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_UrbFab</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.661072210654841</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1.082462090244562e-08</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Comm</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-1.210354256597059</v>
-      </c>
-      <c r="C23" t="n">
-        <v>2.734992471001247e-15</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>transit_accessibility</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.0001789587965853143</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1.919170433349788e-40</v>
+        <v>4.368646679140848e-40</v>
       </c>
     </row>
   </sheetData>
@@ -769,7 +691,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -801,296 +723,218 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.022475992890223</v>
+        <v>-0.5723597746878057</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4718352230045585</v>
+        <v>0.001127780789953415</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult]</t>
+          <t>Country[T.Germany]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.583035986070435</v>
+        <v>-0.7173262553469617</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2614955471514322</v>
+        <v>4.277472599204902e-50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult_Kids]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.734368646331906</v>
+        <v>0.2679606930497986</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2190416511832886</v>
+        <v>5.885709141041236e-74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female]</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5504344788505537</v>
+        <v>0.0005537781835669572</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6963089360545711</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9378770441111858</v>
+        <v>0.01532952652914456</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5060510457948848</v>
+        <v>2.025597672914532e-39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Parent]</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.060893368310597</v>
+        <v>-0.006893913923818294</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4521559338524799</v>
+        <v>0.8303107015339661</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Country[T.Germany]</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.8486372118436607</v>
+        <v>0.455898906133381</v>
       </c>
       <c r="C8" t="n">
-        <v>2.350967222271369e-64</v>
+        <v>9.247716902940899e-22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.02842167236812294</v>
+        <v>0.2512047604292436</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3357777769851982</v>
+        <v>4.693758758842634e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004861212933406949</v>
+        <v>-7.393640505225261e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>3.355594370909813e-289</v>
+        <v>1.337810155011957e-123</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01444720974840216</v>
+        <v>-0.002996422993214211</v>
       </c>
       <c r="C11" t="n">
-        <v>6.448964974328022e-33</v>
+        <v>0.7474169050601591</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.009225089129273473</v>
+        <v>-0.001479648844044016</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7778036368314571</v>
+        <v>0.7437693453180163</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.528397384108945</v>
+        <v>0.0820878217554398</v>
       </c>
       <c r="C13" t="n">
-        <v>3.174045312557394e-28</v>
+        <v>0.6103850492810758</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3057680874930103</v>
+        <v>-0.001718723755044257</v>
       </c>
       <c r="C14" t="n">
-        <v>1.228554014715592e-06</v>
+        <v>0.1849649436728709</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7.713716064099475e-05</v>
+        <v>-0.001505616927056063</v>
       </c>
       <c r="C15" t="n">
-        <v>1.555153656430617e-92</v>
+        <v>0.1150093694784154</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.074184358970783e-08</v>
+        <v>0.7517496645974486</v>
       </c>
       <c r="C16" t="n">
-        <v>0.003563818417034432</v>
+        <v>4.095594326660027e-11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.002057141670451132</v>
+        <v>-0.8737601285386167</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8279676509928717</v>
+        <v>8.26927905006956e-10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>transit_accessibility</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.0006212083049087506</v>
+        <v>-0.0001492303061830467</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8925628858507831</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>bike_lane_share</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.308250268067228</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.05690063259143426</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>IntersecDensity</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.001615426314141976</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.2198084340694451</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>street_length</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>-0.001290460161353794</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.1912270874367248</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_UrbFab</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.6684057429233667</v>
-      </c>
-      <c r="C22" t="n">
-        <v>8.525380625354256e-09</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Comm</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-1.205104480627759</v>
-      </c>
-      <c r="C23" t="n">
-        <v>4.314246704666007e-15</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>transit_accessibility</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.000174823221423499</v>
-      </c>
-      <c r="C24" t="n">
-        <v>3.914573348104679e-39</v>
+        <v>4.565760017681255e-38</v>
       </c>
     </row>
   </sheetData>
@@ -1104,7 +948,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1136,296 +980,218 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.622463284711719</v>
+        <v>-0.5297793073223211</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7072611481372567</v>
+        <v>0.002561505674844388</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult]</t>
+          <t>Country[T.Germany]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.164548573955199</v>
+        <v>-0.7018494222266797</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4797124928842759</v>
+        <v>3.988512597765208e-48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult_Kids]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.355762204747555</v>
+        <v>0.2690223724333405</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4109330841118189</v>
+        <v>4.777338929643867e-75</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female]</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1259761800822501</v>
+        <v>0.0005612352459882313</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9390715174603523</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.4851074345386527</v>
+        <v>0.01503109799270765</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7685075990569715</v>
+        <v>5.216691278113855e-38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Parent]</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6465909624313141</v>
+        <v>-0.008050384184414665</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6949489858113511</v>
+        <v>0.8029137696211667</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Country[T.Germany]</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.8136664715459839</v>
+        <v>0.463093681162367</v>
       </c>
       <c r="C8" t="n">
-        <v>8.117959679931654e-60</v>
+        <v>1.156959302905089e-22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.04349720617814885</v>
+        <v>0.2703717831983549</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1401254946180658</v>
+        <v>1.098803416597022e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004810834903972462</v>
+        <v>-7.640676670794148e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>1.262900626576428e-282</v>
+        <v>4.914239206689794e-130</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01474458446202221</v>
+        <v>-0.0006300429294284808</v>
       </c>
       <c r="C11" t="n">
-        <v>2.446536293364742e-34</v>
+        <v>0.9458139850331481</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.01316084391657876</v>
+        <v>-0.005784446988109105</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6872111956695518</v>
+        <v>0.1993745525152811</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4998872471230455</v>
+        <v>0.1250373733855454</v>
       </c>
       <c r="C13" t="n">
-        <v>1.245650930927302e-25</v>
+        <v>0.4399632288311531</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.2910275978529063</v>
+        <v>-0.002568821541267764</v>
       </c>
       <c r="C14" t="n">
-        <v>3.595224178012416e-06</v>
+        <v>0.04756828275296406</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7.733813815257415e-05</v>
+        <v>-0.001661895161492062</v>
       </c>
       <c r="C15" t="n">
-        <v>1.300032866537027e-92</v>
+        <v>0.08259166217894162</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.581823512993497e-08</v>
+        <v>0.8327073435594498</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0002942539243297428</v>
+        <v>2.59720634672091e-13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.01114712678188161</v>
+        <v>-0.9314076582468637</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2396169414333829</v>
+        <v>5.386359811859892e-11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>transit_accessibility</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001606577072794545</v>
+        <v>-0.0001405011253916078</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9721316879941401</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>bike_lane_share</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.2646447314426945</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.1040660474242158</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>IntersecDensity</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.001102456741958006</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.4021878454963116</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>street_length</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>-0.001341521610858711</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.1697851717526319</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_UrbFab</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.6731229577434782</v>
-      </c>
-      <c r="C22" t="n">
-        <v>6.410811169276279e-09</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Comm</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-1.196366545037327</v>
-      </c>
-      <c r="C23" t="n">
-        <v>5.795374078772386e-15</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>transit_accessibility</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.0001848140732706664</v>
-      </c>
-      <c r="C24" t="n">
-        <v>8.470456769456095e-43</v>
+        <v>1.300555390814508e-33</v>
       </c>
     </row>
   </sheetData>
@@ -1439,7 +1205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1471,296 +1237,218 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.108951117544164</v>
+        <v>-0.4325611789958879</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4344363158718599</v>
+        <v>0.01354749259566806</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult]</t>
+          <t>Country[T.Germany]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.628446200584726</v>
+        <v>-0.7408239354036779</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2473195647820532</v>
+        <v>9.25142960781232e-54</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult_Kids]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.807457038000365</v>
+        <v>0.2718111331456377</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1995309602518228</v>
+        <v>4.437104298832461e-77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female]</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5746347516738786</v>
+        <v>0.0005546708494676982</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6831945354115091</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9736895330122503</v>
+        <v>0.01441408466287309</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4892633561224869</v>
+        <v>3.654335236258528e-35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Parent]</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.123834196782086</v>
+        <v>0.001004000272191082</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4250466235541777</v>
+        <v>0.9750254869360625</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Country[T.Germany]</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.8221523423905066</v>
+        <v>0.4274545486619332</v>
       </c>
       <c r="C8" t="n">
-        <v>8.083304185820746e-61</v>
+        <v>1.162240057883673e-19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.0339999829398434</v>
+        <v>0.2523520360745941</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2485530805158338</v>
+        <v>4.007229136479312e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004876392666140225</v>
+        <v>-7.351768745161256e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>4.635228066917371e-290</v>
+        <v>4.226769746528282e-122</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01419282315983517</v>
+        <v>-0.005296316333123504</v>
       </c>
       <c r="C11" t="n">
-        <v>6.970933211550011e-32</v>
+        <v>0.5670163693396901</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.002315215442629448</v>
+        <v>-0.002786561209770855</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9435273321798616</v>
+        <v>0.5347650277340031</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4662352149603596</v>
+        <v>0.1354871655189276</v>
       </c>
       <c r="C13" t="n">
-        <v>2.363648485751643e-22</v>
+        <v>0.4004598819316778</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3008513227352874</v>
+        <v>-0.002431499214496102</v>
       </c>
       <c r="C14" t="n">
-        <v>1.845832496482499e-06</v>
+        <v>0.0596007255361997</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7.695113722269813e-05</v>
+        <v>-0.001631854211910512</v>
       </c>
       <c r="C15" t="n">
-        <v>4.45185717341096e-92</v>
+        <v>0.08921128219202583</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.873101370360357e-08</v>
+        <v>0.6857912238491447</v>
       </c>
       <c r="C16" t="n">
-        <v>0.008368905372701737</v>
+        <v>1.377835970258771e-09</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.008105486048780853</v>
+        <v>-0.9420944937599589</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3918016849928576</v>
+        <v>2.641833628133616e-11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>transit_accessibility</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.001290146763840585</v>
+        <v>-0.0001409990325555337</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7786180499844347</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>bike_lane_share</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.3725151743229417</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.02163660221107662</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>IntersecDensity</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.0009502994217398863</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.4694906649867625</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>street_length</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>-0.001251054017830815</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.2008019940793606</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_UrbFab</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.6945735007944286</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1.981178212511066e-09</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Comm</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-1.097460199708997</v>
-      </c>
-      <c r="C23" t="n">
-        <v>8.719337219737067e-13</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>transit_accessibility</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.0001765775775091535</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1.248748110021758e-39</v>
+        <v>3.113356238800076e-34</v>
       </c>
     </row>
   </sheetData>
@@ -1774,7 +1462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1806,284 +1494,218 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-28.46809034319133</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
+        <v>-0.5489525265961865</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.001821245167639951</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult]</t>
+          <t>Country[T.Germany]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>29.03841432270555</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
+        <v>-0.7314365935889794</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.178816923365277e-52</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult_Kids]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>29.15690812883869</v>
-      </c>
-      <c r="C4" t="inlineStr"/>
+        <v>0.2669406191780123</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.79675722465614e-74</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female]</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>27.98738863838122</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
+        <v>0.0005567854142492614</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28.37235903472307</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
+        <v>0.01447597174874726</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.330250771234179e-35</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Parent]</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>28.4877423102871</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
+        <v>0.009423747515508231</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.7695624940147495</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Country[T.Germany]</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.8283153807083494</v>
+        <v>0.4321039226910582</v>
       </c>
       <c r="C8" t="n">
-        <v>9.368710036030815e-62</v>
+        <v>4.090594937860414e-20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.02300866316031533</v>
+        <v>0.276292912512595</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4313278177833774</v>
+        <v>6.71378651243961e-06</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004808277686214723</v>
+        <v>-7.371253122204404e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>7.436476925039774e-285</v>
+        <v>1.90695891462606e-123</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01398457507250907</v>
+        <v>0.00306239022005571</v>
       </c>
       <c r="C11" t="n">
-        <v>4.564959746513483e-31</v>
+        <v>0.7420697240380849</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.002485006310660529</v>
+        <v>-0.002085155323700609</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9392693252666795</v>
+        <v>0.6433379040527473</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5170209393412551</v>
+        <v>0.1828082060590868</v>
       </c>
       <c r="C13" t="n">
-        <v>3.084295882172442e-27</v>
+        <v>0.2547482626867302</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3351842942247951</v>
+        <v>-0.001850591824078012</v>
       </c>
       <c r="C14" t="n">
-        <v>9.991119716831552e-08</v>
+        <v>0.1522139618678412</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7.602306112168593e-05</v>
+        <v>-0.001077728697250524</v>
       </c>
       <c r="C15" t="n">
-        <v>9.86363640568001e-89</v>
+        <v>0.2628643647957197</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.388006530204737e-08</v>
+        <v>0.6400772192484706</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0007649632963454688</v>
+        <v>1.826607470752866e-08</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.009771858232912402</v>
+        <v>-0.933109826810772</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3015370354828917</v>
+        <v>5.558730101143993e-11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>transit_accessibility</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.0007965157340349538</v>
+        <v>-0.0001421629220725379</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8622001138887637</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>bike_lane_share</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.2491088097277364</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.126055199088332</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>IntersecDensity</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.001337422708866199</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.3099891401283047</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>street_length</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>-0.001658190000411166</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.09039821165589808</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_UrbFab</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.694151198447302</v>
-      </c>
-      <c r="C22" t="n">
-        <v>2.145168629436351e-09</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Comm</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-1.153693302495795</v>
-      </c>
-      <c r="C23" t="n">
-        <v>4.965903152903661e-14</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>transit_accessibility</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.0001855596339611006</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1.511125335654539e-43</v>
+        <v>6.5120922785501e-35</v>
       </c>
     </row>
   </sheetData>
@@ -2097,7 +1719,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2129,296 +1751,218 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.088341061838423</v>
+        <v>-0.625242274589604</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4435490485105852</v>
+        <v>0.000406692875062926</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult]</t>
+          <t>Country[T.Germany]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.606928562953589</v>
+        <v>-0.7477320945423763</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2541557203112242</v>
+        <v>7.412738984637329e-54</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult_Kids]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.673405870066591</v>
+        <v>0.2754755497829738</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2354658705661351</v>
+        <v>2.836086451349162e-78</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female]</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.590732990233482</v>
+        <v>0.0005608702608983177</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6751678986413501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9596712764506419</v>
+        <v>0.01589064038445654</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4960284518063918</v>
+        <v>5.335382133395116e-42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Parent]</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.084504941076865</v>
+        <v>0.007509739015826594</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4419580341509299</v>
+        <v>0.8160893103053104</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Country[T.Germany]</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.8284957497511133</v>
+        <v>0.4386971294165222</v>
       </c>
       <c r="C8" t="n">
-        <v>1.114261699185942e-61</v>
+        <v>2.344298436819059e-20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0074249272523275</v>
+        <v>0.2580313116120422</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8040721933633687</v>
+        <v>2.94281866878637e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004878454473127166</v>
+        <v>-7.415234867924438e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>5.241684941174502e-289</v>
+        <v>8.631092010717079e-124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01415500879204543</v>
+        <v>0.001883960226837155</v>
       </c>
       <c r="C11" t="n">
-        <v>1.166388635279311e-31</v>
+        <v>0.8399116545440908</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.01359351816670298</v>
+        <v>-0.005365130293044498</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6775372580098606</v>
+        <v>0.2374593018239193</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5097106304097569</v>
+        <v>0.09764316485119881</v>
       </c>
       <c r="C13" t="n">
-        <v>1.814510107123465e-26</v>
+        <v>0.544106901273032</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3128130806350046</v>
+        <v>-0.0015439821033426</v>
       </c>
       <c r="C14" t="n">
-        <v>6.554223217066243e-07</v>
+        <v>0.2367844302358555</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7.71216004836064e-05</v>
+        <v>-0.001087358545159975</v>
       </c>
       <c r="C15" t="n">
-        <v>1.051229967194337e-92</v>
+        <v>0.2601335510325891</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.168577161135596e-08</v>
+        <v>0.7382413258667124</v>
       </c>
       <c r="C16" t="n">
-        <v>0.002258722477606421</v>
+        <v>1.132460583398889e-10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.007984760823532448</v>
+        <v>-0.9698911215719717</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4008646032919267</v>
+        <v>9.585130168606182e-12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>transit_accessibility</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.001795696057901278</v>
+        <v>-0.0001481048150179896</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6966013915294403</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>bike_lane_share</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.2986880278120171</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.06636610488561709</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>IntersecDensity</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.001412947145769287</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.2831149953605639</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>street_length</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>-0.001698469913043791</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.08311472979399859</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_UrbFab</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.6708835192431952</v>
-      </c>
-      <c r="C22" t="n">
-        <v>7.455283709898299e-09</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Comm</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-1.190092052897126</v>
-      </c>
-      <c r="C23" t="n">
-        <v>8.770505187517743e-15</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>transit_accessibility</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.00017329767932195</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1.313549353110381e-38</v>
+        <v>1.484593161574477e-37</v>
       </c>
     </row>
   </sheetData>
@@ -2432,7 +1976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2464,296 +2008,218 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.060841011491677</v>
+        <v>-0.5869068949396299</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4554398889957257</v>
+        <v>0.0008976819286294489</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult]</t>
+          <t>Country[T.Germany]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.618530459459186</v>
+        <v>-0.6995394347838343</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2510757693232718</v>
+        <v>9.713957923829352e-48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult_Kids]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.771403008202022</v>
+        <v>0.2650271092330198</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2094798806992129</v>
+        <v>8.044767289978094e-73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female]</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5675320224542622</v>
+        <v>0.000557242640802639</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6874437955190402</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9460548108527647</v>
+        <v>0.0152869049042616</v>
       </c>
       <c r="C6" t="n">
-        <v>0.502460178063538</v>
+        <v>4.123420612556425e-39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Parent]</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.09082334372643</v>
+        <v>0.00278031309310617</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4396204007695659</v>
+        <v>0.9313715672448852</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Country[T.Germany]</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.8250800285890103</v>
+        <v>0.436033788560939</v>
       </c>
       <c r="C8" t="n">
-        <v>4.94936129596331e-61</v>
+        <v>2.842920742163748e-20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.02672955876264855</v>
+        <v>0.2438580451570478</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3666297311528107</v>
+        <v>7.656174467078032e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004836907981627833</v>
+        <v>-7.340840096820226e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>1.931389739559004e-285</v>
+        <v>9.317195473964559e-122</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01425441519993058</v>
+        <v>0.003208614513580738</v>
       </c>
       <c r="C11" t="n">
-        <v>3.423900268060974e-32</v>
+        <v>0.7313107289634104</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.01335778906624994</v>
+        <v>4.426099323030006e-05</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6828305718398906</v>
+        <v>0.9922018148996525</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5188227736165916</v>
+        <v>0.1004033391712892</v>
       </c>
       <c r="C13" t="n">
-        <v>2.649995339726155e-27</v>
+        <v>0.5340220903245507</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3328068626266619</v>
+        <v>-0.001011762848476662</v>
       </c>
       <c r="C14" t="n">
-        <v>1.274075167848017e-07</v>
+        <v>0.4369648691115976</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7.763878623630445e-05</v>
+        <v>-0.001477983723025801</v>
       </c>
       <c r="C15" t="n">
-        <v>1.951040741143973e-93</v>
+        <v>0.1261069606798999</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.95204207297796e-08</v>
+        <v>0.694755564670186</v>
       </c>
       <c r="C16" t="n">
-        <v>0.005904576363726781</v>
+        <v>1.191295403950025e-09</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.006076384851990939</v>
+        <v>-0.950128966157063</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5225298380956672</v>
+        <v>2.673173211331852e-11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>transit_accessibility</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.0002563635789285029</v>
+        <v>-0.0001509469030547844</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9553611954676906</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>bike_lane_share</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.2281862701842575</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.1602534320937321</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>IntersecDensity</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.0002932419969330209</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.8238904135554164</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>street_length</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>-0.001428249349951232</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.1418221570133838</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_UrbFab</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.5971156678864238</v>
-      </c>
-      <c r="C22" t="n">
-        <v>2.51706708886753e-07</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Comm</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-1.146436580156372</v>
-      </c>
-      <c r="C23" t="n">
-        <v>8.311771733589428e-14</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>transit_accessibility</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.0001774498600636285</v>
-      </c>
-      <c r="C24" t="n">
-        <v>3.264024303269504e-40</v>
+        <v>1.039887056416007e-38</v>
       </c>
     </row>
   </sheetData>
@@ -2767,7 +2233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2799,296 +2265,218 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.102891224688956</v>
+        <v>-0.6636879955117178</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4383435351618082</v>
+        <v>0.0001669002425897764</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult]</t>
+          <t>Country[T.Germany]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.613213472575682</v>
+        <v>-0.7280870107181695</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2531550389645875</v>
+        <v>3.032707040491359e-51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult_Kids]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.783441223756919</v>
+        <v>0.2695890045978619</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2068946013398573</v>
+        <v>1.269645862468019e-75</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female]</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5321793678790409</v>
+        <v>0.0005559532873827051</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7062831303927399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9143068712738945</v>
+        <v>0.01531212714392995</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5173622142012453</v>
+        <v>2.127590360793821e-39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Parent]</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.078865843548172</v>
+        <v>-0.006117859926894948</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4451485427498356</v>
+        <v>0.8493554327663371</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Country[T.Germany]</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.8478919733632494</v>
+        <v>0.4528687126425802</v>
       </c>
       <c r="C8" t="n">
-        <v>4.435960364977608e-64</v>
+        <v>7.396658768735029e-22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.04427275025978826</v>
+        <v>0.2586508901508566</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1324484572100501</v>
+        <v>2.592775228403507e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004884866885343882</v>
+        <v>-7.582051892951087e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>3.602194771021698e-289</v>
+        <v>8.514095636285544e-129</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01426664798303888</v>
+        <v>-0.001222664888235178</v>
       </c>
       <c r="C11" t="n">
-        <v>3.906875833469504e-32</v>
+        <v>0.8954350399258617</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.004932162833952558</v>
+        <v>-0.003113757826031773</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8805472791881324</v>
+        <v>0.4908651714002287</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5126534168113008</v>
+        <v>0.1820776459287044</v>
       </c>
       <c r="C13" t="n">
-        <v>9.854475060856266e-27</v>
+        <v>0.257735259077686</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3236238460424135</v>
+        <v>-0.001321075766113523</v>
       </c>
       <c r="C14" t="n">
-        <v>2.793232340666403e-07</v>
+        <v>0.3083978509403533</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7.674465089036031e-05</v>
+        <v>-0.0007910909842603633</v>
       </c>
       <c r="C15" t="n">
-        <v>4.653763890408996e-91</v>
+        <v>0.4128601095913895</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.994594675950803e-08</v>
+        <v>0.7896160217279988</v>
       </c>
       <c r="C16" t="n">
-        <v>0.004922266807242191</v>
+        <v>4.694849162254841e-12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.01233431909731635</v>
+        <v>-0.9206965221834237</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1951946082497084</v>
+        <v>9.380138777558315e-11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>transit_accessibility</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.001566220067108571</v>
+        <v>-0.0001457960723787971</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7339233001793781</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>bike_lane_share</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.2445835456608992</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.1338890954203465</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>IntersecDensity</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.0007196400572894832</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.5869991678051889</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>street_length</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>-0.0009516264553643894</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.3394366803174638</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_UrbFab</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.6733440032947234</v>
-      </c>
-      <c r="C22" t="n">
-        <v>6.540660922684899e-09</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Comm</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-1.170688356684088</v>
-      </c>
-      <c r="C23" t="n">
-        <v>3.606145027882505e-14</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>transit_accessibility</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.0001731473544755639</v>
-      </c>
-      <c r="C24" t="n">
-        <v>6.612498921884387e-38</v>
+        <v>2.279039396442739e-36</v>
       </c>
     </row>
   </sheetData>
@@ -3102,7 +2490,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3134,296 +2522,218 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.084909728588816</v>
+        <v>-0.6383250304759538</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4454389416684585</v>
+        <v>0.0003072105521230909</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult]</t>
+          <t>Country[T.Germany]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.599101749948994</v>
+        <v>-0.7157664471233026</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2569599732844408</v>
+        <v>1.36003676263793e-49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HHType_simp[T.MultiAdult_Kids]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.765836030424812</v>
+        <v>0.2813848036804336</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2110585006395701</v>
+        <v>9.437987044995375e-81</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female]</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5469012589436452</v>
+        <v>0.0005626161336010463</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6983271771958799</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9136260152231419</v>
+        <v>0.01459129717873419</v>
       </c>
       <c r="C6" t="n">
-        <v>0.517351476892898</v>
+        <v>6.513102395306273e-36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Parent]</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.076668506652808</v>
+        <v>0.009502108169899302</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4457173595429486</v>
+        <v>0.7679423730656902</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Country[T.Germany]</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.8439888797632132</v>
+        <v>0.4361673090222985</v>
       </c>
       <c r="C8" t="n">
-        <v>2.819591605639396e-63</v>
+        <v>2.857825852170453e-20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.03907401501485499</v>
+        <v>0.2777279255845769</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1860129327959411</v>
+        <v>6.437127730101366e-06</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004871086032374137</v>
+        <v>-7.421226053821615e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>1.470073751526222e-289</v>
+        <v>6.80914842316314e-124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01396913634317891</v>
+        <v>0.001553932027956476</v>
       </c>
       <c r="C11" t="n">
-        <v>8.380583290906567e-31</v>
+        <v>0.8671874290545766</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.01899074265951978</v>
+        <v>-0.003182155749840416</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5614173769579078</v>
+        <v>0.4830240724779011</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5358394939983525</v>
+        <v>0.1932880467703638</v>
       </c>
       <c r="C13" t="n">
-        <v>6.936827897911433e-29</v>
+        <v>0.231345343530812</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3378980008306247</v>
+        <v>-0.001311847742320332</v>
       </c>
       <c r="C14" t="n">
-        <v>7.956267433382433e-08</v>
+        <v>0.3125435875560182</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7.886880900801572e-05</v>
+        <v>-0.001039063779111723</v>
       </c>
       <c r="C15" t="n">
-        <v>1.213839251365638e-96</v>
+        <v>0.2829726750624304</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.870716400512222e-08</v>
+        <v>0.7449806300746143</v>
       </c>
       <c r="C16" t="n">
-        <v>6.02096277939178e-05</v>
+        <v>7.195680242941085e-11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.0122214437184114</v>
+        <v>-0.9625077671346441</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1990815069610141</v>
+        <v>1.364617531462113e-11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>transit_accessibility</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.001590053087210656</v>
+        <v>-0.000150219370560077</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7297397288806556</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>bike_lane_share</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.2506944799292412</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.1233300397031097</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>IntersecDensity</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.0009141002590637268</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.4886245546832745</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>street_length</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>-0.0008700046644784304</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.3755764113654789</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_UrbFab</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.6870418546359559</v>
-      </c>
-      <c r="C22" t="n">
-        <v>3.143538832804019e-09</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Comm</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-1.251760264462901</v>
-      </c>
-      <c r="C23" t="n">
-        <v>3.781616965604384e-16</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>transit_accessibility</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.0001866948329455228</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1.782266923083796e-44</v>
+        <v>2.262984041408988e-38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun pooled models with normalized d2c
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/carown_LR_new/All.xlsx
+++ b/outputs/ML_Results/carown_LR_new/All.xlsx
@@ -7,15 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summ11" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="summ4" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summ2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summ5" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="summ3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="summ6" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="summ1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="summ13" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="summ5" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="summ0" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="summ10" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="summ0" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="summ14" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="summ1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="summ4" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="summ7" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="summ11" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -466,10 +466,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.6792876572187736</v>
+        <v>-0.918999159934639</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0001154037508087015</v>
+        <v>3.467030490610146e-07</v>
       </c>
     </row>
     <row r="3">
@@ -479,10 +479,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.6932928383871587</v>
+        <v>-0.6033865476785383</v>
       </c>
       <c r="C3" t="n">
-        <v>7.389768819826593e-47</v>
+        <v>3.219578827003218e-38</v>
       </c>
     </row>
     <row r="4">
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.265190506434564</v>
+        <v>0.2738140163022489</v>
       </c>
       <c r="C4" t="n">
-        <v>2.862631531377701e-73</v>
+        <v>1.590199377767316e-77</v>
       </c>
     </row>
     <row r="5">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005603425989494482</v>
+        <v>0.0005550828642443791</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -518,10 +518,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01518467287388999</v>
+        <v>0.01386435498940276</v>
       </c>
       <c r="C6" t="n">
-        <v>9.898582073376447e-39</v>
+        <v>1.715239838836841e-32</v>
       </c>
     </row>
     <row r="7">
@@ -531,10 +531,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.01909577362631367</v>
+        <v>0.009005470086171615</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5525966870532008</v>
+        <v>0.7803609577960849</v>
       </c>
     </row>
     <row r="8">
@@ -544,10 +544,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4207491837138595</v>
+        <v>0.4475724572348374</v>
       </c>
       <c r="C8" t="n">
-        <v>4.923493323300056e-19</v>
+        <v>3.956609165367508e-21</v>
       </c>
     </row>
     <row r="9">
@@ -557,10 +557,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2460489416724882</v>
+        <v>0.2919163640731889</v>
       </c>
       <c r="C9" t="n">
-        <v>6.490934952455066e-05</v>
+        <v>2.303554398906974e-06</v>
       </c>
     </row>
     <row r="10">
@@ -570,10 +570,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.398088470586898e-05</v>
+        <v>-7.388605036827405e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>8.321799084141013e-123</v>
+        <v>7.678372064705444e-123</v>
       </c>
     </row>
     <row r="11">
@@ -583,23 +583,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.006649625420101253</v>
+        <v>-0.01263658547111004</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4760156776144464</v>
+        <v>0.179205660948899</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>DistCenter_pc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.001578298991352138</v>
+        <v>0.002923176953791801</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7271301704805967</v>
+        <v>1.130049007761167e-13</v>
       </c>
     </row>
     <row r="13">
@@ -609,10 +609,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1927770932598639</v>
+        <v>0.3608054233951324</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2308065717258432</v>
+        <v>0.0250341209765402</v>
       </c>
     </row>
     <row r="14">
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.001075451042636122</v>
+        <v>0.0002855739853420207</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4075118299921993</v>
+        <v>0.8259856284524387</v>
       </c>
     </row>
     <row r="15">
@@ -635,10 +635,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001160357900432417</v>
+        <v>-0.002751817709267548</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2276299366658003</v>
+        <v>0.002966542320272509</v>
       </c>
     </row>
     <row r="16">
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7798484611914137</v>
+        <v>0.6968912964808137</v>
       </c>
       <c r="C16" t="n">
-        <v>8.123662600689844e-12</v>
+        <v>4.211046784362147e-10</v>
       </c>
     </row>
     <row r="17">
@@ -661,10 +661,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.9138947773743836</v>
+        <v>-0.6982253027379975</v>
       </c>
       <c r="C17" t="n">
-        <v>1.111752971516955e-10</v>
+        <v>1.440743358917774e-06</v>
       </c>
     </row>
     <row r="18">
@@ -674,10 +674,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.000153784295390177</v>
+        <v>-0.0001214450241088899</v>
       </c>
       <c r="C18" t="n">
-        <v>4.368646679140848e-40</v>
+        <v>2.45551165690393e-24</v>
       </c>
     </row>
   </sheetData>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.5723597746878057</v>
+        <v>-0.837617338224926</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001127780789953415</v>
+        <v>3.615707302873595e-06</v>
       </c>
     </row>
     <row r="3">
@@ -736,10 +736,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.7173262553469617</v>
+        <v>-0.611058413498311</v>
       </c>
       <c r="C3" t="n">
-        <v>4.277472599204902e-50</v>
+        <v>2.34636671918417e-39</v>
       </c>
     </row>
     <row r="4">
@@ -749,10 +749,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2679606930497986</v>
+        <v>0.2722684947427278</v>
       </c>
       <c r="C4" t="n">
-        <v>5.885709141041236e-74</v>
+        <v>3.31695878060707e-76</v>
       </c>
     </row>
     <row r="5">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005537781835669572</v>
+        <v>0.0005587833371663015</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -775,10 +775,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01532952652914456</v>
+        <v>0.01424753398559522</v>
       </c>
       <c r="C6" t="n">
-        <v>2.025597672914532e-39</v>
+        <v>2.943560178067979e-34</v>
       </c>
     </row>
     <row r="7">
@@ -788,10 +788,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.006893913923818294</v>
+        <v>0.006038888346354018</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8303107015339661</v>
+        <v>0.8519120162813656</v>
       </c>
     </row>
     <row r="8">
@@ -801,10 +801,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.455898906133381</v>
+        <v>0.4445102255348063</v>
       </c>
       <c r="C8" t="n">
-        <v>9.247716902940899e-22</v>
+        <v>4.998527594035003e-21</v>
       </c>
     </row>
     <row r="9">
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2512047604292436</v>
+        <v>0.2691466994409506</v>
       </c>
       <c r="C9" t="n">
-        <v>4.693758758842634e-05</v>
+        <v>1.218072574974409e-05</v>
       </c>
     </row>
     <row r="10">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.393640505225261e-05</v>
+        <v>-7.182037502243807e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>1.337810155011957e-123</v>
+        <v>4.996248766852013e-117</v>
       </c>
     </row>
     <row r="11">
@@ -840,23 +840,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.002996422993214211</v>
+        <v>-0.01752797909861065</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7474169050601591</v>
+        <v>0.06127067369075299</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>DistCenter_pc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.001479648844044016</v>
+        <v>0.003139176823171713</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7437693453180163</v>
+        <v>1.741223540817838e-15</v>
       </c>
     </row>
     <row r="13">
@@ -866,10 +866,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.0820878217554398</v>
+        <v>0.3826342143493172</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6103850492810758</v>
+        <v>0.01758870333264658</v>
       </c>
     </row>
     <row r="14">
@@ -879,10 +879,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.001718723755044257</v>
+        <v>-0.0002268717019910899</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1849649436728709</v>
+        <v>0.8614532158547316</v>
       </c>
     </row>
     <row r="15">
@@ -892,10 +892,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001505616927056063</v>
+        <v>-0.00353677922781616</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1150093694784154</v>
+        <v>0.0001461778679695982</v>
       </c>
     </row>
     <row r="16">
@@ -905,10 +905,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7517496645974486</v>
+        <v>0.6829990125643406</v>
       </c>
       <c r="C16" t="n">
-        <v>4.095594326660027e-11</v>
+        <v>8.680891679157355e-10</v>
       </c>
     </row>
     <row r="17">
@@ -918,10 +918,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.8737601285386167</v>
+        <v>-0.6928338298643026</v>
       </c>
       <c r="C17" t="n">
-        <v>8.26927905006956e-10</v>
+        <v>1.666570542899262e-06</v>
       </c>
     </row>
     <row r="18">
@@ -931,10 +931,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001492303061830467</v>
+        <v>-0.00012130071689933</v>
       </c>
       <c r="C18" t="n">
-        <v>4.565760017681255e-38</v>
+        <v>1.526224422646137e-24</v>
       </c>
     </row>
   </sheetData>
@@ -980,10 +980,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.5297793073223211</v>
+        <v>-0.7894135675120735</v>
       </c>
       <c r="C2" t="n">
-        <v>0.002561505674844388</v>
+        <v>1.226303129966875e-05</v>
       </c>
     </row>
     <row r="3">
@@ -993,10 +993,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.7018494222266797</v>
+        <v>-0.6083459829862496</v>
       </c>
       <c r="C3" t="n">
-        <v>3.988512597765208e-48</v>
+        <v>7.534186862319907e-39</v>
       </c>
     </row>
     <row r="4">
@@ -1006,10 +1006,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2690223724333405</v>
+        <v>0.2621947778310082</v>
       </c>
       <c r="C4" t="n">
-        <v>4.777338929643867e-75</v>
+        <v>1.554772839863902e-70</v>
       </c>
     </row>
     <row r="5">
@@ -1019,7 +1019,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005612352459882313</v>
+        <v>0.0005550559109987965</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -1032,10 +1032,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01503109799270765</v>
+        <v>0.01370337354242208</v>
       </c>
       <c r="C6" t="n">
-        <v>5.216691278113855e-38</v>
+        <v>8.61833715057318e-32</v>
       </c>
     </row>
     <row r="7">
@@ -1045,10 +1045,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.008050384184414665</v>
+        <v>0.0282600651470394</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8029137696211667</v>
+        <v>0.3805590286858336</v>
       </c>
     </row>
     <row r="8">
@@ -1058,10 +1058,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.463093681162367</v>
+        <v>0.421757262518809</v>
       </c>
       <c r="C8" t="n">
-        <v>1.156959302905089e-22</v>
+        <v>5.139633367548454e-19</v>
       </c>
     </row>
     <row r="9">
@@ -1071,10 +1071,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2703717831983549</v>
+        <v>0.2502392483217661</v>
       </c>
       <c r="C9" t="n">
-        <v>1.098803416597022e-05</v>
+        <v>4.694980231305827e-05</v>
       </c>
     </row>
     <row r="10">
@@ -1084,10 +1084,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.640676670794148e-05</v>
+        <v>-7.47378767072789e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>4.914239206689794e-130</v>
+        <v>2.249142366656074e-126</v>
       </c>
     </row>
     <row r="11">
@@ -1097,23 +1097,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.0006300429294284808</v>
+        <v>-0.01855241632509</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9458139850331481</v>
+        <v>0.04746767010511512</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>DistCenter_pc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.005784446988109105</v>
+        <v>0.003039899154072705</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1993745525152811</v>
+        <v>1.06129319162436e-14</v>
       </c>
     </row>
     <row r="13">
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1250373733855454</v>
+        <v>0.2443229333261155</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4399632288311531</v>
+        <v>0.1284584807416608</v>
       </c>
     </row>
     <row r="14">
@@ -1136,10 +1136,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.002568821541267764</v>
+        <v>0.0004411498214823105</v>
       </c>
       <c r="C14" t="n">
-        <v>0.04756828275296406</v>
+        <v>0.7335518072400298</v>
       </c>
     </row>
     <row r="15">
@@ -1149,10 +1149,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001661895161492062</v>
+        <v>-0.003042819628520567</v>
       </c>
       <c r="C15" t="n">
-        <v>0.08259166217894162</v>
+        <v>0.001101994099780205</v>
       </c>
     </row>
     <row r="16">
@@ -1162,10 +1162,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.8327073435594498</v>
+        <v>0.6198244452414531</v>
       </c>
       <c r="C16" t="n">
-        <v>2.59720634672091e-13</v>
+        <v>2.512938616691911e-08</v>
       </c>
     </row>
     <row r="17">
@@ -1175,10 +1175,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.9314076582468637</v>
+        <v>-0.7754940171949163</v>
       </c>
       <c r="C17" t="n">
-        <v>5.386359811859892e-11</v>
+        <v>7.622434552164802e-08</v>
       </c>
     </row>
     <row r="18">
@@ -1188,10 +1188,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001405011253916078</v>
+        <v>-0.0001121687615573495</v>
       </c>
       <c r="C18" t="n">
-        <v>1.300555390814508e-33</v>
+        <v>3.121743941084366e-21</v>
       </c>
     </row>
   </sheetData>
@@ -1237,10 +1237,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.4325611789958879</v>
+        <v>-1.058210621547087</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01354749259566806</v>
+        <v>4.269454761387866e-09</v>
       </c>
     </row>
     <row r="3">
@@ -1250,10 +1250,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.7408239354036779</v>
+        <v>-0.5982576794899733</v>
       </c>
       <c r="C3" t="n">
-        <v>9.25142960781232e-54</v>
+        <v>5.868709551871192e-38</v>
       </c>
     </row>
     <row r="4">
@@ -1263,10 +1263,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2718111331456377</v>
+        <v>0.2618964512557267</v>
       </c>
       <c r="C4" t="n">
-        <v>4.437104298832461e-77</v>
+        <v>1.327922054937891e-71</v>
       </c>
     </row>
     <row r="5">
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005546708494676982</v>
+        <v>0.0005543082273815208</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -1289,10 +1289,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01441408466287309</v>
+        <v>0.01488547853727818</v>
       </c>
       <c r="C6" t="n">
-        <v>3.654335236258528e-35</v>
+        <v>2.342221879477096e-37</v>
       </c>
     </row>
     <row r="7">
@@ -1302,10 +1302,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001004000272191082</v>
+        <v>0.02690095012268427</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9750254869360625</v>
+        <v>0.4042189415694231</v>
       </c>
     </row>
     <row r="8">
@@ -1315,10 +1315,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4274545486619332</v>
+        <v>0.4306835253381808</v>
       </c>
       <c r="C8" t="n">
-        <v>1.162240057883673e-19</v>
+        <v>7.316782011111174e-20</v>
       </c>
     </row>
     <row r="9">
@@ -1328,10 +1328,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2523520360745941</v>
+        <v>0.2364469947448964</v>
       </c>
       <c r="C9" t="n">
-        <v>4.007229136479312e-05</v>
+        <v>0.0001203378144384555</v>
       </c>
     </row>
     <row r="10">
@@ -1341,10 +1341,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.351768745161256e-05</v>
+        <v>-7.375396913576599e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>4.226769746528282e-122</v>
+        <v>1.589797006219889e-123</v>
       </c>
     </row>
     <row r="11">
@@ -1354,23 +1354,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.005296316333123504</v>
+        <v>-0.01411993576464326</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5670163693396901</v>
+        <v>0.1306779273328625</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>DistCenter_pc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.002786561209770855</v>
+        <v>0.003132610485043581</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5347650277340031</v>
+        <v>1.159875405354209e-15</v>
       </c>
     </row>
     <row r="13">
@@ -1380,10 +1380,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1354871655189276</v>
+        <v>0.4240050243833402</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4004598819316778</v>
+        <v>0.008487060769297916</v>
       </c>
     </row>
     <row r="14">
@@ -1393,10 +1393,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.002431499214496102</v>
+        <v>0.0009047269917179097</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0596007255361997</v>
+        <v>0.4858056734474153</v>
       </c>
     </row>
     <row r="15">
@@ -1406,10 +1406,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001631854211910512</v>
+        <v>-0.002391299024627629</v>
       </c>
       <c r="C15" t="n">
-        <v>0.08921128219202583</v>
+        <v>0.009970042866253711</v>
       </c>
     </row>
     <row r="16">
@@ -1419,10 +1419,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6857912238491447</v>
+        <v>0.6815411612933205</v>
       </c>
       <c r="C16" t="n">
-        <v>1.377835970258771e-09</v>
+        <v>8.062271162743384e-10</v>
       </c>
     </row>
     <row r="17">
@@ -1432,10 +1432,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.9420944937599589</v>
+        <v>-0.617924624439722</v>
       </c>
       <c r="C17" t="n">
-        <v>2.641833628133616e-11</v>
+        <v>1.807900102246248e-05</v>
       </c>
     </row>
     <row r="18">
@@ -1445,10 +1445,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001409990325555337</v>
+        <v>-0.0001176565290370418</v>
       </c>
       <c r="C18" t="n">
-        <v>3.113356238800076e-34</v>
+        <v>2.948447323737908e-23</v>
       </c>
     </row>
   </sheetData>
@@ -1494,10 +1494,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.5489525265961865</v>
+        <v>-0.8479098035826894</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001821245167639951</v>
+        <v>2.719245574702528e-06</v>
       </c>
     </row>
     <row r="3">
@@ -1507,10 +1507,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.7314365935889794</v>
+        <v>-0.6004508124568247</v>
       </c>
       <c r="C3" t="n">
-        <v>3.178816923365277e-52</v>
+        <v>4.979910803543046e-38</v>
       </c>
     </row>
     <row r="4">
@@ -1520,10 +1520,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2669406191780123</v>
+        <v>0.2649290981427551</v>
       </c>
       <c r="C4" t="n">
-        <v>1.79675722465614e-74</v>
+        <v>6.787727647662161e-73</v>
       </c>
     </row>
     <row r="5">
@@ -1533,7 +1533,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005567854142492614</v>
+        <v>0.0005631358988335549</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -1546,10 +1546,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01447597174874726</v>
+        <v>0.0145505858332803</v>
       </c>
       <c r="C6" t="n">
-        <v>1.330250771234179e-35</v>
+        <v>1.194903393616621e-35</v>
       </c>
     </row>
     <row r="7">
@@ -1559,10 +1559,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.009423747515508231</v>
+        <v>0.01653527670301403</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7695624940147495</v>
+        <v>0.6086000537814176</v>
       </c>
     </row>
     <row r="8">
@@ -1572,10 +1572,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4321039226910582</v>
+        <v>0.4114069667369277</v>
       </c>
       <c r="C8" t="n">
-        <v>4.090594937860414e-20</v>
+        <v>3.047826779731331e-18</v>
       </c>
     </row>
     <row r="9">
@@ -1585,10 +1585,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.276292912512595</v>
+        <v>0.2461229014766139</v>
       </c>
       <c r="C9" t="n">
-        <v>6.71378651243961e-06</v>
+        <v>6.565866191086085e-05</v>
       </c>
     </row>
     <row r="10">
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.371253122204404e-05</v>
+        <v>-7.136891985176123e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>1.90695891462606e-123</v>
+        <v>3.762361201660085e-115</v>
       </c>
     </row>
     <row r="11">
@@ -1611,23 +1611,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.00306239022005571</v>
+        <v>-0.01347359141652811</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7420697240380849</v>
+        <v>0.1494395297487696</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>DistCenter_pc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.002085155323700609</v>
+        <v>0.002864863674671316</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6433379040527473</v>
+        <v>2.874390645768452e-13</v>
       </c>
     </row>
     <row r="13">
@@ -1637,10 +1637,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1828082060590868</v>
+        <v>0.3074639580037099</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2547482626867302</v>
+        <v>0.05627744285071855</v>
       </c>
     </row>
     <row r="14">
@@ -1650,10 +1650,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.001850591824078012</v>
+        <v>0.0001972859198704869</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1522139618678412</v>
+        <v>0.8793325961656545</v>
       </c>
     </row>
     <row r="15">
@@ -1663,10 +1663,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001077728697250524</v>
+        <v>-0.003174692911759593</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2628643647957197</v>
+        <v>0.0006428386938627715</v>
       </c>
     </row>
     <row r="16">
@@ -1676,10 +1676,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6400772192484706</v>
+        <v>0.6395313844347545</v>
       </c>
       <c r="C16" t="n">
-        <v>1.826607470752866e-08</v>
+        <v>9.38386687271762e-09</v>
       </c>
     </row>
     <row r="17">
@@ -1689,10 +1689,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.933109826810772</v>
+        <v>-0.7059977701810454</v>
       </c>
       <c r="C17" t="n">
-        <v>5.558730101143993e-11</v>
+        <v>1.088753176064531e-06</v>
       </c>
     </row>
     <row r="18">
@@ -1702,10 +1702,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001421629220725379</v>
+        <v>-0.0001274056540285724</v>
       </c>
       <c r="C18" t="n">
-        <v>6.5120922785501e-35</v>
+        <v>1.133521154138466e-26</v>
       </c>
     </row>
   </sheetData>
@@ -1751,10 +1751,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.625242274589604</v>
+        <v>-0.8399777772111321</v>
       </c>
       <c r="C2" t="n">
-        <v>0.000406692875062926</v>
+        <v>3.331066930497672e-06</v>
       </c>
     </row>
     <row r="3">
@@ -1764,10 +1764,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.7477320945423763</v>
+        <v>-0.6045428841982204</v>
       </c>
       <c r="C3" t="n">
-        <v>7.412738984637329e-54</v>
+        <v>1.268259004585874e-38</v>
       </c>
     </row>
     <row r="4">
@@ -1777,10 +1777,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2754755497829738</v>
+        <v>0.270323617363815</v>
       </c>
       <c r="C4" t="n">
-        <v>2.836086451349162e-78</v>
+        <v>4.559004585468925e-75</v>
       </c>
     </row>
     <row r="5">
@@ -1790,7 +1790,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005608702608983177</v>
+        <v>0.0005528550058776156</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -1803,10 +1803,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01589064038445654</v>
+        <v>0.01395772403569527</v>
       </c>
       <c r="C6" t="n">
-        <v>5.335382133395116e-42</v>
+        <v>6.486979691358955e-33</v>
       </c>
     </row>
     <row r="7">
@@ -1816,10 +1816,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.007509739015826594</v>
+        <v>0.01188042354963206</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8160893103053104</v>
+        <v>0.7124788660224685</v>
       </c>
     </row>
     <row r="8">
@@ -1829,10 +1829,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4386971294165222</v>
+        <v>0.4442370785574933</v>
       </c>
       <c r="C8" t="n">
-        <v>2.344298436819059e-20</v>
+        <v>5.791745432460907e-21</v>
       </c>
     </row>
     <row r="9">
@@ -1842,10 +1842,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2580313116120422</v>
+        <v>0.2648906864191955</v>
       </c>
       <c r="C9" t="n">
-        <v>2.94281866878637e-05</v>
+        <v>1.697875304120486e-05</v>
       </c>
     </row>
     <row r="10">
@@ -1855,10 +1855,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.415234867924438e-05</v>
+        <v>-7.56490167155446e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>8.631092010717079e-124</v>
+        <v>5.349923669723877e-129</v>
       </c>
     </row>
     <row r="11">
@@ -1868,23 +1868,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.001883960226837155</v>
+        <v>-0.01591785176280035</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8399116545440908</v>
+        <v>0.08771295679694188</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>DistCenter_pc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.005365130293044498</v>
+        <v>0.003093248777190072</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2374593018239193</v>
+        <v>3.324265003319426e-15</v>
       </c>
     </row>
     <row r="13">
@@ -1894,10 +1894,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.09764316485119881</v>
+        <v>0.3127625660232409</v>
       </c>
       <c r="C13" t="n">
-        <v>0.544106901273032</v>
+        <v>0.05237979571465906</v>
       </c>
     </row>
     <row r="14">
@@ -1907,10 +1907,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.0015439821033426</v>
+        <v>3.30781514064416e-05</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2367844302358555</v>
+        <v>0.9796588606411736</v>
       </c>
     </row>
     <row r="15">
@@ -1920,10 +1920,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001087358545159975</v>
+        <v>-0.003036914322533199</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2601335510325891</v>
+        <v>0.001047262707183866</v>
       </c>
     </row>
     <row r="16">
@@ -1933,10 +1933,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7382413258667124</v>
+        <v>0.6490487636068379</v>
       </c>
       <c r="C16" t="n">
-        <v>1.132460583398889e-10</v>
+        <v>5.371052273617567e-09</v>
       </c>
     </row>
     <row r="17">
@@ -1946,10 +1946,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.9698911215719717</v>
+        <v>-0.7866249506715034</v>
       </c>
       <c r="C17" t="n">
-        <v>9.585130168606182e-12</v>
+        <v>4.826902590865766e-08</v>
       </c>
     </row>
     <row r="18">
@@ -1959,10 +1959,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001481048150179896</v>
+        <v>-0.0001088860848965803</v>
       </c>
       <c r="C18" t="n">
-        <v>1.484593161574477e-37</v>
+        <v>4.052033020188418e-20</v>
       </c>
     </row>
   </sheetData>
@@ -2008,10 +2008,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.5869068949396299</v>
+        <v>-0.8060665207448</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0008976819286294489</v>
+        <v>7.701025247060786e-06</v>
       </c>
     </row>
     <row r="3">
@@ -2021,10 +2021,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.6995394347838343</v>
+        <v>-0.6126103114087215</v>
       </c>
       <c r="C3" t="n">
-        <v>9.713957923829352e-48</v>
+        <v>1.117207352013746e-39</v>
       </c>
     </row>
     <row r="4">
@@ -2034,10 +2034,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2650271092330198</v>
+        <v>0.2560224266135858</v>
       </c>
       <c r="C4" t="n">
-        <v>8.044767289978094e-73</v>
+        <v>9.599551121967038e-69</v>
       </c>
     </row>
     <row r="5">
@@ -2047,7 +2047,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.000557242640802639</v>
+        <v>0.0005530239856163506</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -2060,10 +2060,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0152869049042616</v>
+        <v>0.01468889528286265</v>
       </c>
       <c r="C6" t="n">
-        <v>4.123420612556425e-39</v>
+        <v>4.244223049928988e-36</v>
       </c>
     </row>
     <row r="7">
@@ -2073,10 +2073,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.00278031309310617</v>
+        <v>0.01110497623448364</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9313715672448852</v>
+        <v>0.7306446901490857</v>
       </c>
     </row>
     <row r="8">
@@ -2086,10 +2086,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.436033788560939</v>
+        <v>0.4005367305424962</v>
       </c>
       <c r="C8" t="n">
-        <v>2.842920742163748e-20</v>
+        <v>3.322567511334661e-17</v>
       </c>
     </row>
     <row r="9">
@@ -2099,10 +2099,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2438580451570478</v>
+        <v>0.2058693213870702</v>
       </c>
       <c r="C9" t="n">
-        <v>7.656174467078032e-05</v>
+        <v>0.0009037176840826875</v>
       </c>
     </row>
     <row r="10">
@@ -2112,10 +2112,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.340840096820226e-05</v>
+        <v>-7.290122764763571e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>9.317195473964559e-122</v>
+        <v>2.575813000244792e-122</v>
       </c>
     </row>
     <row r="11">
@@ -2125,23 +2125,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.003208614513580738</v>
+        <v>-0.01805989759582185</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7313107289634104</v>
+        <v>0.0536019010231162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>DistCenter_pc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.426099323030006e-05</v>
+        <v>0.003162130698799338</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9922018148996525</v>
+        <v>9.020536982885302e-16</v>
       </c>
     </row>
     <row r="13">
@@ -2151,10 +2151,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1004033391712892</v>
+        <v>0.330023249505822</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5340220903245507</v>
+        <v>0.04126986562042712</v>
       </c>
     </row>
     <row r="14">
@@ -2164,10 +2164,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.001011762848476662</v>
+        <v>-0.0005189237429694363</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4369648691115976</v>
+        <v>0.6889159180922912</v>
       </c>
     </row>
     <row r="15">
@@ -2177,10 +2177,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001477983723025801</v>
+        <v>-0.00332137826370959</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1261069606798999</v>
+        <v>0.0003145473298549379</v>
       </c>
     </row>
     <row r="16">
@@ -2190,10 +2190,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.694755564670186</v>
+        <v>0.7631851527544099</v>
       </c>
       <c r="C16" t="n">
-        <v>1.191295403950025e-09</v>
+        <v>6.863549269091877e-12</v>
       </c>
     </row>
     <row r="17">
@@ -2203,10 +2203,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.950128966157063</v>
+        <v>-0.6900235554972473</v>
       </c>
       <c r="C17" t="n">
-        <v>2.673173211331852e-11</v>
+        <v>1.69850862854673e-06</v>
       </c>
     </row>
     <row r="18">
@@ -2216,10 +2216,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001509469030547844</v>
+        <v>-0.0001191759559142829</v>
       </c>
       <c r="C18" t="n">
-        <v>1.039887056416007e-38</v>
+        <v>2.642987032890147e-24</v>
       </c>
     </row>
   </sheetData>
@@ -2265,10 +2265,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.6636879955117178</v>
+        <v>-0.8901039084776312</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0001669002425897764</v>
+        <v>8.342227721776364e-07</v>
       </c>
     </row>
     <row r="3">
@@ -2278,10 +2278,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.7280870107181695</v>
+        <v>-0.5962650984661652</v>
       </c>
       <c r="C3" t="n">
-        <v>3.032707040491359e-51</v>
+        <v>2.18499004803133e-37</v>
       </c>
     </row>
     <row r="4">
@@ -2291,10 +2291,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2695890045978619</v>
+        <v>0.2672607125980139</v>
       </c>
       <c r="C4" t="n">
-        <v>1.269645862468019e-75</v>
+        <v>6.998880923574463e-74</v>
       </c>
     </row>
     <row r="5">
@@ -2304,7 +2304,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005559532873827051</v>
+        <v>0.0005513307950651353</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -2317,10 +2317,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01531212714392995</v>
+        <v>0.01469059266029172</v>
       </c>
       <c r="C6" t="n">
-        <v>2.127590360793821e-39</v>
+        <v>3.719189914840156e-36</v>
       </c>
     </row>
     <row r="7">
@@ -2330,10 +2330,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.006117859926894948</v>
+        <v>0.02755426675814544</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8493554327663371</v>
+        <v>0.3941904312220663</v>
       </c>
     </row>
     <row r="8">
@@ -2343,10 +2343,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4528687126425802</v>
+        <v>0.3954890889703349</v>
       </c>
       <c r="C8" t="n">
-        <v>7.396658768735029e-22</v>
+        <v>4.783125189560556e-17</v>
       </c>
     </row>
     <row r="9">
@@ -2356,10 +2356,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2586508901508566</v>
+        <v>0.2134671759740532</v>
       </c>
       <c r="C9" t="n">
-        <v>2.592775228403507e-05</v>
+        <v>0.00051601258597522</v>
       </c>
     </row>
     <row r="10">
@@ -2369,10 +2369,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.582051892951087e-05</v>
+        <v>-7.29366948489388e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>8.514095636285544e-129</v>
+        <v>1.560276284713305e-120</v>
       </c>
     </row>
     <row r="11">
@@ -2382,23 +2382,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.001222664888235178</v>
+        <v>-0.004904135117995615</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8954350399258617</v>
+        <v>0.6028104871244787</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>DistCenter_pc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.003113757826031773</v>
+        <v>0.002891614951326176</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4908651714002287</v>
+        <v>2.896288462037426e-13</v>
       </c>
     </row>
     <row r="13">
@@ -2408,10 +2408,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1820776459287044</v>
+        <v>0.2765176719126062</v>
       </c>
       <c r="C13" t="n">
-        <v>0.257735259077686</v>
+        <v>0.08574553890718964</v>
       </c>
     </row>
     <row r="14">
@@ -2421,10 +2421,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.001321075766113523</v>
+        <v>0.0005972246062727779</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3083978509403533</v>
+        <v>0.6457236344819248</v>
       </c>
     </row>
     <row r="15">
@@ -2434,10 +2434,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.0007910909842603633</v>
+        <v>-0.002812937462276646</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4128601095913895</v>
+        <v>0.002440694989020094</v>
       </c>
     </row>
     <row r="16">
@@ -2447,10 +2447,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7896160217279988</v>
+        <v>0.6426963435896189</v>
       </c>
       <c r="C16" t="n">
-        <v>4.694849162254841e-12</v>
+        <v>7.915728862684651e-09</v>
       </c>
     </row>
     <row r="17">
@@ -2460,10 +2460,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.9206965221834237</v>
+        <v>-0.7601018489828213</v>
       </c>
       <c r="C17" t="n">
-        <v>9.380138777558315e-11</v>
+        <v>1.348232282191691e-07</v>
       </c>
     </row>
     <row r="18">
@@ -2473,10 +2473,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001457960723787971</v>
+        <v>-0.0001180597180504275</v>
       </c>
       <c r="C18" t="n">
-        <v>2.279039396442739e-36</v>
+        <v>2.202841061086458e-23</v>
       </c>
     </row>
   </sheetData>
@@ -2522,10 +2522,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.6383250304759538</v>
+        <v>-0.9691620992946459</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0003072105521230909</v>
+        <v>8.684254542024193e-08</v>
       </c>
     </row>
     <row r="3">
@@ -2535,10 +2535,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.7157664471233026</v>
+        <v>-0.6002884406178015</v>
       </c>
       <c r="C3" t="n">
-        <v>1.36003676263793e-49</v>
+        <v>4.960359009080482e-38</v>
       </c>
     </row>
     <row r="4">
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2813848036804336</v>
+        <v>0.2684881602706329</v>
       </c>
       <c r="C4" t="n">
-        <v>9.437987044995375e-81</v>
+        <v>1.675894374697703e-74</v>
       </c>
     </row>
     <row r="5">
@@ -2561,7 +2561,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005626161336010463</v>
+        <v>0.0005567191647261914</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -2574,10 +2574,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01459129717873419</v>
+        <v>0.01460714688124717</v>
       </c>
       <c r="C6" t="n">
-        <v>6.513102395306273e-36</v>
+        <v>1.273538001538045e-35</v>
       </c>
     </row>
     <row r="7">
@@ -2587,10 +2587,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.009502108169899302</v>
+        <v>-0.001910809745769942</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7679423730656902</v>
+        <v>0.9529037183664893</v>
       </c>
     </row>
     <row r="8">
@@ -2600,10 +2600,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4361673090222985</v>
+        <v>0.4349137635537532</v>
       </c>
       <c r="C8" t="n">
-        <v>2.857825852170453e-20</v>
+        <v>4.726778913077635e-20</v>
       </c>
     </row>
     <row r="9">
@@ -2613,10 +2613,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2777279255845769</v>
+        <v>0.2388011744689241</v>
       </c>
       <c r="C9" t="n">
-        <v>6.437127730101366e-06</v>
+        <v>0.0001159568046882343</v>
       </c>
     </row>
     <row r="10">
@@ -2626,10 +2626,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.421226053821615e-05</v>
+        <v>-7.501059248109855e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>6.80914842316314e-124</v>
+        <v>1.764785413028245e-126</v>
       </c>
     </row>
     <row r="11">
@@ -2639,23 +2639,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.001553932027956476</v>
+        <v>-0.01715428219868326</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8671874290545766</v>
+        <v>0.06732419727577339</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>DistCenter_pc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.003182155749840416</v>
+        <v>0.003033585615399961</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4830240724779011</v>
+        <v>1.424784660138011e-14</v>
       </c>
     </row>
     <row r="13">
@@ -2665,10 +2665,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1932880467703638</v>
+        <v>0.3013213163249902</v>
       </c>
       <c r="C13" t="n">
-        <v>0.231345343530812</v>
+        <v>0.06248345445839483</v>
       </c>
     </row>
     <row r="14">
@@ -2678,10 +2678,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.001311847742320332</v>
+        <v>0.0007205302232867176</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3125435875560182</v>
+        <v>0.5783701990343826</v>
       </c>
     </row>
     <row r="15">
@@ -2691,10 +2691,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001039063779111723</v>
+        <v>-0.002454218019098535</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2829726750624304</v>
+        <v>0.008464634534762748</v>
       </c>
     </row>
     <row r="16">
@@ -2704,10 +2704,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7449806300746143</v>
+        <v>0.7183972075373899</v>
       </c>
       <c r="C16" t="n">
-        <v>7.195680242941085e-11</v>
+        <v>1.229677497641433e-10</v>
       </c>
     </row>
     <row r="17">
@@ -2717,10 +2717,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.9625077671346441</v>
+        <v>-0.7079330061843138</v>
       </c>
       <c r="C17" t="n">
-        <v>1.364617531462113e-11</v>
+        <v>1.062129872388704e-06</v>
       </c>
     </row>
     <row r="18">
@@ -2730,10 +2730,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.000150219370560077</v>
+        <v>-0.0001199039006267585</v>
       </c>
       <c r="C18" t="n">
-        <v>2.262984041408988e-38</v>
+        <v>1.1630012086518e-23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun of models including new transit access feature
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/carown_LR_new/All.xlsx
+++ b/outputs/ML_Results/carown_LR_new/All.xlsx
@@ -7,15 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summ2" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="summ5" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summ7" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summ8" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="summ3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="summ0" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="summ14" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="summ1" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="summ4" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="summ7" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="summ11" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="summ1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="summ4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="summ11" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="summ21" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="summ0" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="summ2" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -466,10 +466,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.918999159934639</v>
+        <v>-0.7869744579494594</v>
       </c>
       <c r="C2" t="n">
-        <v>3.467030490610146e-07</v>
+        <v>1.234709371738346e-05</v>
       </c>
     </row>
     <row r="3">
@@ -479,10 +479,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.6033865476785383</v>
+        <v>-0.4612274065783553</v>
       </c>
       <c r="C3" t="n">
-        <v>3.219578827003218e-38</v>
+        <v>3.130156049470402e-21</v>
       </c>
     </row>
     <row r="4">
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2738140163022489</v>
+        <v>0.2733787342545802</v>
       </c>
       <c r="C4" t="n">
-        <v>1.590199377767316e-77</v>
+        <v>8.072407561116971e-77</v>
       </c>
     </row>
     <row r="5">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005550828642443791</v>
+        <v>0.0005510139998898955</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -518,10 +518,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01386435498940276</v>
+        <v>0.01429077704096082</v>
       </c>
       <c r="C6" t="n">
-        <v>1.715239838836841e-32</v>
+        <v>3.056261551966601e-34</v>
       </c>
     </row>
     <row r="7">
@@ -531,10 +531,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.009005470086171615</v>
+        <v>0.02802711075431268</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7803609577960849</v>
+        <v>0.3864621540653459</v>
       </c>
     </row>
     <row r="8">
@@ -544,10 +544,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4475724572348374</v>
+        <v>0.4266093360578351</v>
       </c>
       <c r="C8" t="n">
-        <v>3.956609165367508e-21</v>
+        <v>2.468879173329872e-19</v>
       </c>
     </row>
     <row r="9">
@@ -557,10 +557,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2919163640731889</v>
+        <v>0.2541575299295959</v>
       </c>
       <c r="C9" t="n">
-        <v>2.303554398906974e-06</v>
+        <v>4.039006997388004e-05</v>
       </c>
     </row>
     <row r="10">
@@ -570,10 +570,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.388605036827405e-05</v>
+        <v>-0.007197273762656223</v>
       </c>
       <c r="C10" t="n">
-        <v>7.678372064705444e-123</v>
+        <v>8.930850556026121e-122</v>
       </c>
     </row>
     <row r="11">
@@ -583,10 +583,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01263658547111004</v>
+        <v>-0.01426060471695567</v>
       </c>
       <c r="C11" t="n">
-        <v>0.179205660948899</v>
+        <v>0.1285119039885024</v>
       </c>
     </row>
     <row r="12">
@@ -596,10 +596,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.002923176953791801</v>
+        <v>0.002539527484932714</v>
       </c>
       <c r="C12" t="n">
-        <v>1.130049007761167e-13</v>
+        <v>2.108284048970852e-10</v>
       </c>
     </row>
     <row r="13">
@@ -609,10 +609,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3608054233951324</v>
+        <v>0.2261643599871426</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0250341209765402</v>
+        <v>0.1532097630042462</v>
       </c>
     </row>
     <row r="14">
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0002855739853420207</v>
+        <v>-0.00139274499845463</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8259856284524387</v>
+        <v>0.2813365655680589</v>
       </c>
     </row>
     <row r="15">
@@ -635,10 +635,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.002751817709267548</v>
+        <v>-0.003736351789695065</v>
       </c>
       <c r="C15" t="n">
-        <v>0.002966542320272509</v>
+        <v>4.774900706627487e-05</v>
       </c>
     </row>
     <row r="16">
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6968912964808137</v>
+        <v>0.7417647620181618</v>
       </c>
       <c r="C16" t="n">
-        <v>4.211046784362147e-10</v>
+        <v>4.243409131045984e-11</v>
       </c>
     </row>
     <row r="17">
@@ -661,10 +661,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.6982253027379975</v>
+        <v>-0.6383002820970933</v>
       </c>
       <c r="C17" t="n">
-        <v>1.440743358917774e-06</v>
+        <v>1.125289106009752e-05</v>
       </c>
     </row>
     <row r="18">
@@ -674,10 +674,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001214450241088899</v>
+        <v>-0.01034891979183356</v>
       </c>
       <c r="C18" t="n">
-        <v>2.45551165690393e-24</v>
+        <v>4.287295770457384e-32</v>
       </c>
     </row>
   </sheetData>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.837617338224926</v>
+        <v>-0.8899288918133154</v>
       </c>
       <c r="C2" t="n">
-        <v>3.615707302873595e-06</v>
+        <v>7.808067563023191e-07</v>
       </c>
     </row>
     <row r="3">
@@ -736,10 +736,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.611058413498311</v>
+        <v>-0.4589266106767482</v>
       </c>
       <c r="C3" t="n">
-        <v>2.34636671918417e-39</v>
+        <v>4.195926567407842e-21</v>
       </c>
     </row>
     <row r="4">
@@ -749,10 +749,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2722684947427278</v>
+        <v>0.2672066107322871</v>
       </c>
       <c r="C4" t="n">
-        <v>3.31695878060707e-76</v>
+        <v>1.02730700286071e-73</v>
       </c>
     </row>
     <row r="5">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005587833371663015</v>
+        <v>0.000560524275186639</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -775,10 +775,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01424753398559522</v>
+        <v>0.01428152916124731</v>
       </c>
       <c r="C6" t="n">
-        <v>2.943560178067979e-34</v>
+        <v>2.98023125991928e-34</v>
       </c>
     </row>
     <row r="7">
@@ -788,10 +788,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.006038888346354018</v>
+        <v>0.02210202846128191</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8519120162813656</v>
+        <v>0.4943064144158917</v>
       </c>
     </row>
     <row r="8">
@@ -801,10 +801,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4445102255348063</v>
+        <v>0.4570721030682004</v>
       </c>
       <c r="C8" t="n">
-        <v>4.998527594035003e-21</v>
+        <v>4.961761287842737e-22</v>
       </c>
     </row>
     <row r="9">
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2691466994409506</v>
+        <v>0.2665637603250579</v>
       </c>
       <c r="C9" t="n">
-        <v>1.218072574974409e-05</v>
+        <v>1.534338220004215e-05</v>
       </c>
     </row>
     <row r="10">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.182037502243807e-05</v>
+        <v>-0.007328607526750699</v>
       </c>
       <c r="C10" t="n">
-        <v>4.996248766852013e-117</v>
+        <v>5.09322244974634e-125</v>
       </c>
     </row>
     <row r="11">
@@ -840,10 +840,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01752797909861065</v>
+        <v>-0.01503816062749248</v>
       </c>
       <c r="C11" t="n">
-        <v>0.06127067369075299</v>
+        <v>0.1083047871095354</v>
       </c>
     </row>
     <row r="12">
@@ -853,10 +853,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.003139176823171713</v>
+        <v>0.002615543888027507</v>
       </c>
       <c r="C12" t="n">
-        <v>1.741223540817838e-15</v>
+        <v>6.773829343342228e-11</v>
       </c>
     </row>
     <row r="13">
@@ -866,10 +866,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3826342143493172</v>
+        <v>0.2985305925867297</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01758870333264658</v>
+        <v>0.06035525205757663</v>
       </c>
     </row>
     <row r="14">
@@ -879,10 +879,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.0002268717019910899</v>
+        <v>-0.001188437582697786</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8614532158547316</v>
+        <v>0.3561880907558447</v>
       </c>
     </row>
     <row r="15">
@@ -892,10 +892,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.00353677922781616</v>
+        <v>-0.003309719013072585</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0001461778679695982</v>
+        <v>0.0003193797835533846</v>
       </c>
     </row>
     <row r="16">
@@ -905,10 +905,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6829990125643406</v>
+        <v>0.7477688553376747</v>
       </c>
       <c r="C16" t="n">
-        <v>8.680891679157355e-10</v>
+        <v>3.094784405308418e-11</v>
       </c>
     </row>
     <row r="17">
@@ -918,10 +918,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.6928338298643026</v>
+        <v>-0.7311751389894852</v>
       </c>
       <c r="C17" t="n">
-        <v>1.666570542899262e-06</v>
+        <v>4.900737233908448e-07</v>
       </c>
     </row>
     <row r="18">
@@ -931,10 +931,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.00012130071689933</v>
+        <v>-0.009653714264673399</v>
       </c>
       <c r="C18" t="n">
-        <v>1.526224422646137e-24</v>
+        <v>6.050381411113297e-28</v>
       </c>
     </row>
   </sheetData>
@@ -980,10 +980,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.7894135675120735</v>
+        <v>-0.8337321720988475</v>
       </c>
       <c r="C2" t="n">
-        <v>1.226303129966875e-05</v>
+        <v>3.410374029930276e-06</v>
       </c>
     </row>
     <row r="3">
@@ -993,10 +993,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.6083459829862496</v>
+        <v>-0.4595088264193735</v>
       </c>
       <c r="C3" t="n">
-        <v>7.534186862319907e-39</v>
+        <v>3.15561982542564e-21</v>
       </c>
     </row>
     <row r="4">
@@ -1006,10 +1006,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2621947778310082</v>
+        <v>0.2632127834851842</v>
       </c>
       <c r="C4" t="n">
-        <v>1.554772839863902e-70</v>
+        <v>2.326480386776966e-72</v>
       </c>
     </row>
     <row r="5">
@@ -1019,7 +1019,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005550559109987965</v>
+        <v>0.000557035831524731</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -1032,10 +1032,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01370337354242208</v>
+        <v>0.01418377263938313</v>
       </c>
       <c r="C6" t="n">
-        <v>8.61833715057318e-32</v>
+        <v>4.962069440785915e-34</v>
       </c>
     </row>
     <row r="7">
@@ -1045,10 +1045,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0282600651470394</v>
+        <v>0.02204074518728802</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3805590286858336</v>
+        <v>0.4943341316939427</v>
       </c>
     </row>
     <row r="8">
@@ -1058,10 +1058,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.421757262518809</v>
+        <v>0.4002557407546103</v>
       </c>
       <c r="C8" t="n">
-        <v>5.139633367548454e-19</v>
+        <v>2.042325175496643e-17</v>
       </c>
     </row>
     <row r="9">
@@ -1071,10 +1071,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2502392483217661</v>
+        <v>0.212498708462796</v>
       </c>
       <c r="C9" t="n">
-        <v>4.694980231305827e-05</v>
+        <v>0.0005643424529447831</v>
       </c>
     </row>
     <row r="10">
@@ -1084,10 +1084,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.47378767072789e-05</v>
+        <v>-0.007345425767177543</v>
       </c>
       <c r="C10" t="n">
-        <v>2.249142366656074e-126</v>
+        <v>2.068599585264917e-126</v>
       </c>
     </row>
     <row r="11">
@@ -1097,10 +1097,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01855241632509</v>
+        <v>-0.009634481718380985</v>
       </c>
       <c r="C11" t="n">
-        <v>0.04746767010511512</v>
+        <v>0.3031373657671498</v>
       </c>
     </row>
     <row r="12">
@@ -1110,10 +1110,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.003039899154072705</v>
+        <v>0.002799949553798135</v>
       </c>
       <c r="C12" t="n">
-        <v>1.06129319162436e-14</v>
+        <v>2.45447939303543e-12</v>
       </c>
     </row>
     <row r="13">
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.2443229333261155</v>
+        <v>0.2784124219143553</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1284584807416608</v>
+        <v>0.07844702376804946</v>
       </c>
     </row>
     <row r="14">
@@ -1136,10 +1136,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0004411498214823105</v>
+        <v>-0.001297659839418061</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7335518072400298</v>
+        <v>0.3134036033479159</v>
       </c>
     </row>
     <row r="15">
@@ -1149,10 +1149,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.003042819628520567</v>
+        <v>-0.003746731012742657</v>
       </c>
       <c r="C15" t="n">
-        <v>0.001101994099780205</v>
+        <v>3.895947006090954e-05</v>
       </c>
     </row>
     <row r="16">
@@ -1162,10 +1162,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6198244452414531</v>
+        <v>0.7916637155795108</v>
       </c>
       <c r="C16" t="n">
-        <v>2.512938616691911e-08</v>
+        <v>1.567680475074011e-12</v>
       </c>
     </row>
     <row r="17">
@@ -1175,10 +1175,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.7754940171949163</v>
+        <v>-0.6055746931554733</v>
       </c>
       <c r="C17" t="n">
-        <v>7.622434552164802e-08</v>
+        <v>2.958841639677566e-05</v>
       </c>
     </row>
     <row r="18">
@@ -1188,10 +1188,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001121687615573495</v>
+        <v>-0.009596749642418115</v>
       </c>
       <c r="C18" t="n">
-        <v>3.121743941084366e-21</v>
+        <v>7.77977238249244e-28</v>
       </c>
     </row>
   </sheetData>
@@ -1237,10 +1237,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.058210621547087</v>
+        <v>-0.8590652416078746</v>
       </c>
       <c r="C2" t="n">
-        <v>4.269454761387866e-09</v>
+        <v>1.871606791863646e-06</v>
       </c>
     </row>
     <row r="3">
@@ -1250,10 +1250,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.5982576794899733</v>
+        <v>-0.4410162017569162</v>
       </c>
       <c r="C3" t="n">
-        <v>5.868709551871192e-38</v>
+        <v>1.270978068249271e-19</v>
       </c>
     </row>
     <row r="4">
@@ -1263,10 +1263,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2618964512557267</v>
+        <v>0.2740519637614918</v>
       </c>
       <c r="C4" t="n">
-        <v>1.327922054937891e-71</v>
+        <v>3.667784667727125e-77</v>
       </c>
     </row>
     <row r="5">
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005543082273815208</v>
+        <v>0.0005521471905234317</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -1289,10 +1289,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01488547853727818</v>
+        <v>0.01432992104280487</v>
       </c>
       <c r="C6" t="n">
-        <v>2.342221879477096e-37</v>
+        <v>1.463965026845428e-34</v>
       </c>
     </row>
     <row r="7">
@@ -1302,10 +1302,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.02690095012268427</v>
+        <v>0.01548504996669004</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4042189415694231</v>
+        <v>0.6321237600956031</v>
       </c>
     </row>
     <row r="8">
@@ -1315,10 +1315,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4306835253381808</v>
+        <v>0.4415614249479856</v>
       </c>
       <c r="C8" t="n">
-        <v>7.316782011111174e-20</v>
+        <v>8.76334484334565e-21</v>
       </c>
     </row>
     <row r="9">
@@ -1328,10 +1328,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2364469947448964</v>
+        <v>0.2547879570148769</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0001203378144384555</v>
+        <v>3.483335203355297e-05</v>
       </c>
     </row>
     <row r="10">
@@ -1341,10 +1341,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.375396913576599e-05</v>
+        <v>-0.007291107714640908</v>
       </c>
       <c r="C10" t="n">
-        <v>1.589797006219889e-123</v>
+        <v>3.089958604663085e-124</v>
       </c>
     </row>
     <row r="11">
@@ -1354,10 +1354,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01411993576464326</v>
+        <v>-0.005444562460575895</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1306779273328625</v>
+        <v>0.5599683096203836</v>
       </c>
     </row>
     <row r="12">
@@ -1367,10 +1367,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.003132610485043581</v>
+        <v>0.00236011470106853</v>
       </c>
       <c r="C12" t="n">
-        <v>1.159875405354209e-15</v>
+        <v>3.189423492557086e-09</v>
       </c>
     </row>
     <row r="13">
@@ -1380,10 +1380,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4240050243833402</v>
+        <v>0.1576602546028148</v>
       </c>
       <c r="C13" t="n">
-        <v>0.008487060769297916</v>
+        <v>0.3191496052121388</v>
       </c>
     </row>
     <row r="14">
@@ -1393,10 +1393,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0009047269917179097</v>
+        <v>-0.0007839690234705519</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4858056734474153</v>
+        <v>0.5445928824295596</v>
       </c>
     </row>
     <row r="15">
@@ -1406,10 +1406,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.002391299024627629</v>
+        <v>-0.003593546969453408</v>
       </c>
       <c r="C15" t="n">
-        <v>0.009970042866253711</v>
+        <v>9.065661453159515e-05</v>
       </c>
     </row>
     <row r="16">
@@ -1419,10 +1419,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6815411612933205</v>
+        <v>0.743475850163099</v>
       </c>
       <c r="C16" t="n">
-        <v>8.062271162743384e-10</v>
+        <v>3.683728657427784e-11</v>
       </c>
     </row>
     <row r="17">
@@ -1432,10 +1432,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.617924624439722</v>
+        <v>-0.6317610963056394</v>
       </c>
       <c r="C17" t="n">
-        <v>1.807900102246248e-05</v>
+        <v>1.33869051944676e-05</v>
       </c>
     </row>
     <row r="18">
@@ -1445,10 +1445,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001176565290370418</v>
+        <v>-0.009890787618858247</v>
       </c>
       <c r="C18" t="n">
-        <v>2.948447323737908e-23</v>
+        <v>2.316724260969915e-29</v>
       </c>
     </row>
   </sheetData>
@@ -1494,10 +1494,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.8479098035826894</v>
+        <v>-0.8763451354462706</v>
       </c>
       <c r="C2" t="n">
-        <v>2.719245574702528e-06</v>
+        <v>1.084014451677064e-06</v>
       </c>
     </row>
     <row r="3">
@@ -1507,10 +1507,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.6004508124568247</v>
+        <v>-0.452137915973133</v>
       </c>
       <c r="C3" t="n">
-        <v>4.979910803543046e-38</v>
+        <v>1.076015412192213e-20</v>
       </c>
     </row>
     <row r="4">
@@ -1520,10 +1520,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2649290981427551</v>
+        <v>0.2610415671905409</v>
       </c>
       <c r="C4" t="n">
-        <v>6.787727647662161e-73</v>
+        <v>2.381172342877919e-71</v>
       </c>
     </row>
     <row r="5">
@@ -1533,7 +1533,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005631358988335549</v>
+        <v>0.0005610236678556152</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -1546,10 +1546,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0145505858332803</v>
+        <v>0.01456992561641133</v>
       </c>
       <c r="C6" t="n">
-        <v>1.194903393616621e-35</v>
+        <v>1.005663664658094e-35</v>
       </c>
     </row>
     <row r="7">
@@ -1559,10 +1559,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.01653527670301403</v>
+        <v>0.02292900688608577</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6086000537814176</v>
+        <v>0.4774419114711584</v>
       </c>
     </row>
     <row r="8">
@@ -1572,10 +1572,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4114069667369277</v>
+        <v>0.4153459883439823</v>
       </c>
       <c r="C8" t="n">
-        <v>3.047826779731331e-18</v>
+        <v>1.060364711879876e-18</v>
       </c>
     </row>
     <row r="9">
@@ -1585,10 +1585,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2461229014766139</v>
+        <v>0.2357780521778561</v>
       </c>
       <c r="C9" t="n">
-        <v>6.565866191086085e-05</v>
+        <v>0.0001283577927245741</v>
       </c>
     </row>
     <row r="10">
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.136891985176123e-05</v>
+        <v>-0.007158295820960246</v>
       </c>
       <c r="C10" t="n">
-        <v>3.762361201660085e-115</v>
+        <v>2.360273943556658e-120</v>
       </c>
     </row>
     <row r="11">
@@ -1611,10 +1611,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01347359141652811</v>
+        <v>-0.01894105939231511</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1494395297487696</v>
+        <v>0.04394669211441895</v>
       </c>
     </row>
     <row r="12">
@@ -1624,10 +1624,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.002864863674671316</v>
+        <v>0.002783880455327748</v>
       </c>
       <c r="C12" t="n">
-        <v>2.874390645768452e-13</v>
+        <v>2.820839845223702e-12</v>
       </c>
     </row>
     <row r="13">
@@ -1637,10 +1637,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3074639580037099</v>
+        <v>0.2480845545905388</v>
       </c>
       <c r="C13" t="n">
-        <v>0.05627744285071855</v>
+        <v>0.1164215590486067</v>
       </c>
     </row>
     <row r="14">
@@ -1650,10 +1650,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0001972859198704869</v>
+        <v>-0.00116914923055268</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8793325961656545</v>
+        <v>0.3626549795639815</v>
       </c>
     </row>
     <row r="15">
@@ -1663,10 +1663,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.003174692911759593</v>
+        <v>-0.003581593828436543</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0006428386938627715</v>
+        <v>9.61891350766297e-05</v>
       </c>
     </row>
     <row r="16">
@@ -1676,10 +1676,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6395313844347545</v>
+        <v>0.802906157128631</v>
       </c>
       <c r="C16" t="n">
-        <v>9.38386687271762e-09</v>
+        <v>8.655413623175638e-13</v>
       </c>
     </row>
     <row r="17">
@@ -1689,10 +1689,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.7059977701810454</v>
+        <v>-0.6338621938831651</v>
       </c>
       <c r="C17" t="n">
-        <v>1.088753176064531e-06</v>
+        <v>1.199754892747574e-05</v>
       </c>
     </row>
     <row r="18">
@@ -1702,10 +1702,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001274056540285724</v>
+        <v>-0.01036321102978775</v>
       </c>
       <c r="C18" t="n">
-        <v>1.133521154138466e-26</v>
+        <v>2.798959747854364e-32</v>
       </c>
     </row>
   </sheetData>
@@ -1751,10 +1751,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.8399777772111321</v>
+        <v>-0.9366413265756688</v>
       </c>
       <c r="C2" t="n">
-        <v>3.331066930497672e-06</v>
+        <v>1.746344681662613e-07</v>
       </c>
     </row>
     <row r="3">
@@ -1764,10 +1764,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.6045428841982204</v>
+        <v>-0.4626579490974058</v>
       </c>
       <c r="C3" t="n">
-        <v>1.268259004585874e-38</v>
+        <v>1.345744628900112e-21</v>
       </c>
     </row>
     <row r="4">
@@ -1777,10 +1777,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.270323617363815</v>
+        <v>0.2685508435226673</v>
       </c>
       <c r="C4" t="n">
-        <v>4.559004585468925e-75</v>
+        <v>2.295301200252951e-74</v>
       </c>
     </row>
     <row r="5">
@@ -1790,7 +1790,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005528550058776156</v>
+        <v>0.0005628756897864534</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -1803,10 +1803,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01395772403569527</v>
+        <v>0.01440386079826874</v>
       </c>
       <c r="C6" t="n">
-        <v>6.486979691358955e-33</v>
+        <v>6.346295426947383e-35</v>
       </c>
     </row>
     <row r="7">
@@ -1816,10 +1816,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.01188042354963206</v>
+        <v>0.01621649677245162</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7124788660224685</v>
+        <v>0.6159381378368345</v>
       </c>
     </row>
     <row r="8">
@@ -1829,10 +1829,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4442370785574933</v>
+        <v>0.4344426646562922</v>
       </c>
       <c r="C8" t="n">
-        <v>5.791745432460907e-21</v>
+        <v>3.84822819125407e-20</v>
       </c>
     </row>
     <row r="9">
@@ -1842,10 +1842,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2648906864191955</v>
+        <v>0.2616546729875125</v>
       </c>
       <c r="C9" t="n">
-        <v>1.697875304120486e-05</v>
+        <v>2.150042948456274e-05</v>
       </c>
     </row>
     <row r="10">
@@ -1855,10 +1855,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.56490167155446e-05</v>
+        <v>-0.00736483130302045</v>
       </c>
       <c r="C10" t="n">
-        <v>5.349923669723877e-129</v>
+        <v>1.116508070457213e-126</v>
       </c>
     </row>
     <row r="11">
@@ -1868,10 +1868,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01591785176280035</v>
+        <v>-0.006182527494945071</v>
       </c>
       <c r="C11" t="n">
-        <v>0.08771295679694188</v>
+        <v>0.5081954800743524</v>
       </c>
     </row>
     <row r="12">
@@ -1881,10 +1881,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.003093248777190072</v>
+        <v>0.002505535276164577</v>
       </c>
       <c r="C12" t="n">
-        <v>3.324265003319426e-15</v>
+        <v>3.356292346780856e-10</v>
       </c>
     </row>
     <row r="13">
@@ -1894,10 +1894,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3127625660232409</v>
+        <v>0.2709564792499201</v>
       </c>
       <c r="C13" t="n">
-        <v>0.05237979571465906</v>
+        <v>0.08761548500115529</v>
       </c>
     </row>
     <row r="14">
@@ -1907,10 +1907,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3.30781514064416e-05</v>
+        <v>-0.0006054500305263128</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9796588606411736</v>
+        <v>0.6385747414786003</v>
       </c>
     </row>
     <row r="15">
@@ -1920,10 +1920,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.003036914322533199</v>
+        <v>-0.003199142678671609</v>
       </c>
       <c r="C15" t="n">
-        <v>0.001047262707183866</v>
+        <v>0.0004410664040590801</v>
       </c>
     </row>
     <row r="16">
@@ -1933,10 +1933,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6490487636068379</v>
+        <v>0.7430742030469307</v>
       </c>
       <c r="C16" t="n">
-        <v>5.371052273617567e-09</v>
+        <v>3.623088801343707e-11</v>
       </c>
     </row>
     <row r="17">
@@ -1946,10 +1946,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.7866249506715034</v>
+        <v>-0.6325564667945281</v>
       </c>
       <c r="C17" t="n">
-        <v>4.826902590865766e-08</v>
+        <v>1.294106799066128e-05</v>
       </c>
     </row>
     <row r="18">
@@ -1959,10 +1959,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001088860848965803</v>
+        <v>-0.01010299864573831</v>
       </c>
       <c r="C18" t="n">
-        <v>4.052033020188418e-20</v>
+        <v>1.527154349527657e-30</v>
       </c>
     </row>
   </sheetData>
@@ -2008,10 +2008,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.8060665207448</v>
+        <v>-0.839105195130887</v>
       </c>
       <c r="C2" t="n">
-        <v>7.701025247060786e-06</v>
+        <v>3.000826507167897e-06</v>
       </c>
     </row>
     <row r="3">
@@ -2021,10 +2021,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.6126103114087215</v>
+        <v>-0.4806519295113576</v>
       </c>
       <c r="C3" t="n">
-        <v>1.117207352013746e-39</v>
+        <v>4.929828975944021e-23</v>
       </c>
     </row>
     <row r="4">
@@ -2034,10 +2034,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2560224266135858</v>
+        <v>0.2704527569480386</v>
       </c>
       <c r="C4" t="n">
-        <v>9.599551121967038e-69</v>
+        <v>2.297726947704454e-75</v>
       </c>
     </row>
     <row r="5">
@@ -2047,7 +2047,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005530239856163506</v>
+        <v>0.0005542724839336745</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -2060,10 +2060,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01468889528286265</v>
+        <v>0.0148648750961178</v>
       </c>
       <c r="C6" t="n">
-        <v>4.244223049928988e-36</v>
+        <v>4.947829083357574e-37</v>
       </c>
     </row>
     <row r="7">
@@ -2073,10 +2073,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.01110497623448364</v>
+        <v>0.01009583533510676</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7306446901490857</v>
+        <v>0.7549663151432929</v>
       </c>
     </row>
     <row r="8">
@@ -2086,10 +2086,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4005367305424962</v>
+        <v>0.4168511682824859</v>
       </c>
       <c r="C8" t="n">
-        <v>3.322567511334661e-17</v>
+        <v>1.335952729150898e-18</v>
       </c>
     </row>
     <row r="9">
@@ -2099,10 +2099,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2058693213870702</v>
+        <v>0.2255103346762967</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0009037176840826875</v>
+        <v>0.0002542392082363264</v>
       </c>
     </row>
     <row r="10">
@@ -2112,10 +2112,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.290122764763571e-05</v>
+        <v>-0.007135011670236778</v>
       </c>
       <c r="C10" t="n">
-        <v>2.575813000244792e-122</v>
+        <v>4.26279472710574e-120</v>
       </c>
     </row>
     <row r="11">
@@ -2125,10 +2125,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01805989759582185</v>
+        <v>-0.01575350140371738</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0536019010231162</v>
+        <v>0.09155509366355345</v>
       </c>
     </row>
     <row r="12">
@@ -2138,10 +2138,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.003162130698799338</v>
+        <v>0.002692926452896422</v>
       </c>
       <c r="C12" t="n">
-        <v>9.020536982885302e-16</v>
+        <v>1.396086438167351e-11</v>
       </c>
     </row>
     <row r="13">
@@ -2151,10 +2151,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.330023249505822</v>
+        <v>0.2586840402228592</v>
       </c>
       <c r="C13" t="n">
-        <v>0.04126986562042712</v>
+        <v>0.1024831893012099</v>
       </c>
     </row>
     <row r="14">
@@ -2164,10 +2164,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.0005189237429694363</v>
+        <v>-0.001755601845052889</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6889159180922912</v>
+        <v>0.1724785233007128</v>
       </c>
     </row>
     <row r="15">
@@ -2177,10 +2177,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.00332137826370959</v>
+        <v>-0.003569389089221619</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0003145473298549379</v>
+        <v>0.0001043027267308167</v>
       </c>
     </row>
     <row r="16">
@@ -2190,10 +2190,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7631851527544099</v>
+        <v>0.7623535664070378</v>
       </c>
       <c r="C16" t="n">
-        <v>6.863549269091877e-12</v>
+        <v>1.04390082609757e-11</v>
       </c>
     </row>
     <row r="17">
@@ -2203,10 +2203,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.6900235554972473</v>
+        <v>-0.5797706687248456</v>
       </c>
       <c r="C17" t="n">
-        <v>1.69850862854673e-06</v>
+        <v>6.519837625363993e-05</v>
       </c>
     </row>
     <row r="18">
@@ -2216,10 +2216,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001191759559142829</v>
+        <v>-0.009938525793753565</v>
       </c>
       <c r="C18" t="n">
-        <v>2.642987032890147e-24</v>
+        <v>6.644611737056388e-30</v>
       </c>
     </row>
   </sheetData>
@@ -2265,10 +2265,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.8901039084776312</v>
+        <v>-0.8994566947784425</v>
       </c>
       <c r="C2" t="n">
-        <v>8.342227721776364e-07</v>
+        <v>5.952143671473374e-07</v>
       </c>
     </row>
     <row r="3">
@@ -2278,10 +2278,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.5962650984661652</v>
+        <v>-0.4631505891388865</v>
       </c>
       <c r="C3" t="n">
-        <v>2.18499004803133e-37</v>
+        <v>1.37345609336805e-21</v>
       </c>
     </row>
     <row r="4">
@@ -2291,10 +2291,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2672607125980139</v>
+        <v>0.2640072829404282</v>
       </c>
       <c r="C4" t="n">
-        <v>6.998880923574463e-74</v>
+        <v>9.84399312030476e-73</v>
       </c>
     </row>
     <row r="5">
@@ -2304,7 +2304,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005513307950651353</v>
+        <v>0.0005605183544956485</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -2317,10 +2317,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01469059266029172</v>
+        <v>0.01448056906300821</v>
       </c>
       <c r="C6" t="n">
-        <v>3.719189914840156e-36</v>
+        <v>2.560832643376155e-35</v>
       </c>
     </row>
     <row r="7">
@@ -2330,10 +2330,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.02755426675814544</v>
+        <v>0.009332762251339234</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3941904312220663</v>
+        <v>0.7722800521179772</v>
       </c>
     </row>
     <row r="8">
@@ -2343,10 +2343,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.3954890889703349</v>
+        <v>0.4405061912083038</v>
       </c>
       <c r="C8" t="n">
-        <v>4.783125189560556e-17</v>
+        <v>9.811533470688369e-21</v>
       </c>
     </row>
     <row r="9">
@@ -2356,10 +2356,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2134671759740532</v>
+        <v>0.253630103776226</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00051601258597522</v>
+        <v>3.67254006673682e-05</v>
       </c>
     </row>
     <row r="10">
@@ -2369,10 +2369,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.29366948489388e-05</v>
+        <v>-0.007079119712595127</v>
       </c>
       <c r="C10" t="n">
-        <v>1.560276284713305e-120</v>
+        <v>3.677066011865704e-118</v>
       </c>
     </row>
     <row r="11">
@@ -2382,10 +2382,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.004904135117995615</v>
+        <v>-0.01586772098342974</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6028104871244787</v>
+        <v>0.08974940598368095</v>
       </c>
     </row>
     <row r="12">
@@ -2395,10 +2395,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.002891614951326176</v>
+        <v>0.002768670109051129</v>
       </c>
       <c r="C12" t="n">
-        <v>2.896288462037426e-13</v>
+        <v>3.627846860922233e-12</v>
       </c>
     </row>
     <row r="13">
@@ -2408,10 +2408,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.2765176719126062</v>
+        <v>0.3243912564837138</v>
       </c>
       <c r="C13" t="n">
-        <v>0.08574553890718964</v>
+        <v>0.04116280262143234</v>
       </c>
     </row>
     <row r="14">
@@ -2421,10 +2421,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0005972246062727779</v>
+        <v>-0.00144974302799404</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6457236344819248</v>
+        <v>0.2604240087705728</v>
       </c>
     </row>
     <row r="15">
@@ -2434,10 +2434,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.002812937462276646</v>
+        <v>-0.003401067711042957</v>
       </c>
       <c r="C15" t="n">
-        <v>0.002440694989020094</v>
+        <v>0.0002200388560724261</v>
       </c>
     </row>
     <row r="16">
@@ -2447,10 +2447,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6426963435896189</v>
+        <v>0.7452104406902983</v>
       </c>
       <c r="C16" t="n">
-        <v>7.915728862684651e-09</v>
+        <v>3.021498249938291e-11</v>
       </c>
     </row>
     <row r="17">
@@ -2460,10 +2460,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.7601018489828213</v>
+        <v>-0.6256719418391967</v>
       </c>
       <c r="C17" t="n">
-        <v>1.348232282191691e-07</v>
+        <v>1.675573507267127e-05</v>
       </c>
     </row>
     <row r="18">
@@ -2473,10 +2473,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001180597180504275</v>
+        <v>-0.009829567612994842</v>
       </c>
       <c r="C18" t="n">
-        <v>2.202841061086458e-23</v>
+        <v>5.683698805434675e-29</v>
       </c>
     </row>
   </sheetData>
@@ -2522,10 +2522,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.9691620992946459</v>
+        <v>-0.932283391296919</v>
       </c>
       <c r="C2" t="n">
-        <v>8.684254542024193e-08</v>
+        <v>2.095708870096528e-07</v>
       </c>
     </row>
     <row r="3">
@@ -2535,10 +2535,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.6002884406178015</v>
+        <v>-0.462878360963472</v>
       </c>
       <c r="C3" t="n">
-        <v>4.960359009080482e-38</v>
+        <v>1.717710000058984e-21</v>
       </c>
     </row>
     <row r="4">
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2684881602706329</v>
+        <v>0.2666901604257232</v>
       </c>
       <c r="C4" t="n">
-        <v>1.675894374697703e-74</v>
+        <v>3.516313928104378e-73</v>
       </c>
     </row>
     <row r="5">
@@ -2561,7 +2561,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0005567191647261914</v>
+        <v>0.0005543059033296629</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -2574,10 +2574,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01460714688124717</v>
+        <v>0.01454237175011964</v>
       </c>
       <c r="C6" t="n">
-        <v>1.273538001538045e-35</v>
+        <v>1.918131869203462e-35</v>
       </c>
     </row>
     <row r="7">
@@ -2587,10 +2587,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.001910809745769942</v>
+        <v>0.01545344989321319</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9529037183664893</v>
+        <v>0.6324889226888672</v>
       </c>
     </row>
     <row r="8">
@@ -2600,10 +2600,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4349137635537532</v>
+        <v>0.4450330839707072</v>
       </c>
       <c r="C8" t="n">
-        <v>4.726778913077635e-20</v>
+        <v>8.558253327625456e-21</v>
       </c>
     </row>
     <row r="9">
@@ -2613,10 +2613,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2388011744689241</v>
+        <v>0.2455148744356977</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0001159568046882343</v>
+        <v>7.481819855525264e-05</v>
       </c>
     </row>
     <row r="10">
@@ -2626,10 +2626,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-7.501059248109855e-05</v>
+        <v>-0.00726461840781216</v>
       </c>
       <c r="C10" t="n">
-        <v>1.764785413028245e-126</v>
+        <v>4.043681229441929e-123</v>
       </c>
     </row>
     <row r="11">
@@ -2639,10 +2639,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01715428219868326</v>
+        <v>-0.01312347821627425</v>
       </c>
       <c r="C11" t="n">
-        <v>0.06732419727577339</v>
+        <v>0.1610220466729539</v>
       </c>
     </row>
     <row r="12">
@@ -2652,10 +2652,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.003033585615399961</v>
+        <v>0.002866957066851108</v>
       </c>
       <c r="C12" t="n">
-        <v>1.424784660138011e-14</v>
+        <v>6.183637021303468e-13</v>
       </c>
     </row>
     <row r="13">
@@ -2665,10 +2665,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3013213163249902</v>
+        <v>0.2480260885862304</v>
       </c>
       <c r="C13" t="n">
-        <v>0.06248345445839483</v>
+        <v>0.1173485402144002</v>
       </c>
     </row>
     <row r="14">
@@ -2678,10 +2678,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0007205302232867176</v>
+        <v>-0.0007054168304685763</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5783701990343826</v>
+        <v>0.5845791083006988</v>
       </c>
     </row>
     <row r="15">
@@ -2691,10 +2691,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.002454218019098535</v>
+        <v>-0.003381127644217484</v>
       </c>
       <c r="C15" t="n">
-        <v>0.008464634534762748</v>
+        <v>0.0002134831547348282</v>
       </c>
     </row>
     <row r="16">
@@ -2704,10 +2704,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7183972075373899</v>
+        <v>0.7629297518448359</v>
       </c>
       <c r="C16" t="n">
-        <v>1.229677497641433e-10</v>
+        <v>1.179882973706246e-11</v>
       </c>
     </row>
     <row r="17">
@@ -2717,10 +2717,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.7079330061843138</v>
+        <v>-0.6448552198819537</v>
       </c>
       <c r="C17" t="n">
-        <v>1.062129872388704e-06</v>
+        <v>9.107658976707365e-06</v>
       </c>
     </row>
     <row r="18">
@@ -2730,10 +2730,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0001199039006267585</v>
+        <v>-0.009599607829807575</v>
       </c>
       <c r="C18" t="n">
-        <v>1.1630012086518e-23</v>
+        <v>1.400196310386173e-27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>